<commit_message>
div avgatr; plus tp minus sl infinity
</commit_message>
<xml_diff>
--- a/wm/Results.xlsx
+++ b/wm/Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pioo\notebooks\wm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB616706-C958-4084-897A-ACADFE3178DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{539B1EA3-0303-4AE2-AE14-049D566BCCB4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="435" xr2:uid="{B6B0453F-83A4-43EC-A328-DC10FEB5BD2E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1508" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1589" uniqueCount="55">
   <si>
     <t>Te_cal</t>
   </si>
@@ -195,6 +195,9 @@
   </si>
   <si>
     <t>test12</t>
+  </si>
+  <si>
+    <t>test12_5</t>
   </si>
   <si>
     <t>test13</t>
@@ -590,13 +593,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBA71D6A-A9B1-42AC-9396-7E4A540CDDDA}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:AC494"/>
+  <dimension ref="A1:AC521"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E454" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E484" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E465" sqref="E465"/>
+      <selection pane="bottomRight" activeCell="S499" sqref="S499"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -34541,7 +34544,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="465" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="465" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A465" t="s">
         <v>53</v>
       </c>
@@ -34554,8 +34557,83 @@
       <c r="D465" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="466" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E465">
+        <v>100</v>
+      </c>
+      <c r="F465">
+        <v>67</v>
+      </c>
+      <c r="G465">
+        <v>99</v>
+      </c>
+      <c r="H465">
+        <v>99.9</v>
+      </c>
+      <c r="I465">
+        <v>100</v>
+      </c>
+      <c r="J465">
+        <v>81.7</v>
+      </c>
+      <c r="K465">
+        <v>15</v>
+      </c>
+      <c r="L465">
+        <v>90.5</v>
+      </c>
+      <c r="M465">
+        <v>5</v>
+      </c>
+      <c r="N465">
+        <v>83.7</v>
+      </c>
+      <c r="O465">
+        <v>6</v>
+      </c>
+      <c r="P465">
+        <v>79.099999999999994</v>
+      </c>
+      <c r="Q465">
+        <v>5</v>
+      </c>
+      <c r="R465">
+        <v>79.8</v>
+      </c>
+      <c r="S465">
+        <v>26</v>
+      </c>
+      <c r="T465">
+        <v>36.200000000000003</v>
+      </c>
+      <c r="U465">
+        <v>16</v>
+      </c>
+      <c r="V465">
+        <v>45.9</v>
+      </c>
+      <c r="W465">
+        <v>5</v>
+      </c>
+      <c r="X465">
+        <v>39.1</v>
+      </c>
+      <c r="Y465">
+        <v>8</v>
+      </c>
+      <c r="Z465">
+        <v>38.9</v>
+      </c>
+      <c r="AA465">
+        <v>7</v>
+      </c>
+      <c r="AB465">
+        <v>41.3</v>
+      </c>
+      <c r="AC465">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="466" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A466" t="s">
         <v>53</v>
       </c>
@@ -34568,8 +34646,71 @@
       <c r="D466" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="467" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E466">
+        <v>99.4</v>
+      </c>
+      <c r="F466">
+        <v>68.2</v>
+      </c>
+      <c r="G466">
+        <v>41.8</v>
+      </c>
+      <c r="H466">
+        <v>99.1</v>
+      </c>
+      <c r="I466">
+        <v>99.6</v>
+      </c>
+      <c r="J466">
+        <v>74</v>
+      </c>
+      <c r="K466">
+        <v>78</v>
+      </c>
+      <c r="L466">
+        <v>77.8</v>
+      </c>
+      <c r="M466">
+        <v>23</v>
+      </c>
+      <c r="N466">
+        <v>85.7</v>
+      </c>
+      <c r="O466">
+        <v>7</v>
+      </c>
+      <c r="P466">
+        <v>85.7</v>
+      </c>
+      <c r="Q466">
+        <v>5</v>
+      </c>
+      <c r="R466">
+        <v>91.1</v>
+      </c>
+      <c r="S466">
+        <v>6</v>
+      </c>
+      <c r="T466">
+        <v>37.6</v>
+      </c>
+      <c r="U466">
+        <v>22</v>
+      </c>
+      <c r="V466">
+        <v>24</v>
+      </c>
+      <c r="W466">
+        <v>26</v>
+      </c>
+      <c r="X466">
+        <v>14.9</v>
+      </c>
+      <c r="Y466">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="467" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A467" t="s">
         <v>53</v>
       </c>
@@ -34582,8 +34723,83 @@
       <c r="D467" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="468" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E467">
+        <v>90.9</v>
+      </c>
+      <c r="F467">
+        <v>71.599999999999994</v>
+      </c>
+      <c r="G467">
+        <v>94.4</v>
+      </c>
+      <c r="H467">
+        <v>99.8</v>
+      </c>
+      <c r="I467">
+        <v>100</v>
+      </c>
+      <c r="J467">
+        <v>97.6</v>
+      </c>
+      <c r="K467">
+        <v>5</v>
+      </c>
+      <c r="L467">
+        <v>84.1</v>
+      </c>
+      <c r="M467">
+        <v>9</v>
+      </c>
+      <c r="N467">
+        <v>86.4</v>
+      </c>
+      <c r="O467">
+        <v>7</v>
+      </c>
+      <c r="P467">
+        <v>82.7</v>
+      </c>
+      <c r="Q467">
+        <v>10</v>
+      </c>
+      <c r="R467">
+        <v>80.400000000000006</v>
+      </c>
+      <c r="S467">
+        <v>7</v>
+      </c>
+      <c r="T467">
+        <v>38.6</v>
+      </c>
+      <c r="U467">
+        <v>14</v>
+      </c>
+      <c r="V467">
+        <v>40.799999999999997</v>
+      </c>
+      <c r="W467">
+        <v>6</v>
+      </c>
+      <c r="X467">
+        <v>41</v>
+      </c>
+      <c r="Y467">
+        <v>5</v>
+      </c>
+      <c r="Z467">
+        <v>32.700000000000003</v>
+      </c>
+      <c r="AA467">
+        <v>21</v>
+      </c>
+      <c r="AB467">
+        <v>34.1</v>
+      </c>
+      <c r="AC467">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="468" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A468" t="s">
         <v>53</v>
       </c>
@@ -34596,8 +34812,83 @@
       <c r="D468" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="469" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E468">
+        <v>100</v>
+      </c>
+      <c r="F468">
+        <v>71.7</v>
+      </c>
+      <c r="G468">
+        <v>100</v>
+      </c>
+      <c r="H468">
+        <v>100</v>
+      </c>
+      <c r="I468">
+        <v>100</v>
+      </c>
+      <c r="J468">
+        <v>77.7</v>
+      </c>
+      <c r="K468">
+        <v>47</v>
+      </c>
+      <c r="L468">
+        <v>77.3</v>
+      </c>
+      <c r="M468">
+        <v>34</v>
+      </c>
+      <c r="N468">
+        <v>75.400000000000006</v>
+      </c>
+      <c r="O468">
+        <v>63</v>
+      </c>
+      <c r="P468">
+        <v>76.5</v>
+      </c>
+      <c r="Q468">
+        <v>39</v>
+      </c>
+      <c r="R468">
+        <v>77</v>
+      </c>
+      <c r="S468">
+        <v>15</v>
+      </c>
+      <c r="T468">
+        <v>52.5</v>
+      </c>
+      <c r="U468">
+        <v>5</v>
+      </c>
+      <c r="V468">
+        <v>40</v>
+      </c>
+      <c r="W468">
+        <v>7</v>
+      </c>
+      <c r="X468">
+        <v>50</v>
+      </c>
+      <c r="Y468">
+        <v>5</v>
+      </c>
+      <c r="Z468">
+        <v>39</v>
+      </c>
+      <c r="AA468">
+        <v>7</v>
+      </c>
+      <c r="AB468">
+        <v>43.6</v>
+      </c>
+      <c r="AC468">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="469" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A469" t="s">
         <v>53</v>
       </c>
@@ -34610,8 +34901,53 @@
       <c r="D469" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="470" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E469">
+        <v>100</v>
+      </c>
+      <c r="F469">
+        <v>71.400000000000006</v>
+      </c>
+      <c r="G469">
+        <v>77.099999999999994</v>
+      </c>
+      <c r="H469">
+        <v>100</v>
+      </c>
+      <c r="I469">
+        <v>100</v>
+      </c>
+      <c r="J469">
+        <v>72</v>
+      </c>
+      <c r="K469">
+        <v>97</v>
+      </c>
+      <c r="L469">
+        <v>72.8</v>
+      </c>
+      <c r="M469">
+        <v>75</v>
+      </c>
+      <c r="N469">
+        <v>82.5</v>
+      </c>
+      <c r="O469">
+        <v>5</v>
+      </c>
+      <c r="P469">
+        <v>79.7</v>
+      </c>
+      <c r="Q469">
+        <v>8</v>
+      </c>
+      <c r="R469">
+        <v>72.2</v>
+      </c>
+      <c r="S469">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="470" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A470" t="s">
         <v>53</v>
       </c>
@@ -34624,8 +34960,71 @@
       <c r="D470" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="471" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E470">
+        <v>100</v>
+      </c>
+      <c r="F470">
+        <v>72.400000000000006</v>
+      </c>
+      <c r="G470">
+        <v>98.5</v>
+      </c>
+      <c r="H470">
+        <v>100</v>
+      </c>
+      <c r="I470">
+        <v>100</v>
+      </c>
+      <c r="J470">
+        <v>77.400000000000006</v>
+      </c>
+      <c r="K470">
+        <v>63</v>
+      </c>
+      <c r="L470">
+        <v>84.8</v>
+      </c>
+      <c r="M470">
+        <v>12</v>
+      </c>
+      <c r="N470">
+        <v>82</v>
+      </c>
+      <c r="O470">
+        <v>8</v>
+      </c>
+      <c r="P470">
+        <v>84.1</v>
+      </c>
+      <c r="Q470">
+        <v>14</v>
+      </c>
+      <c r="R470">
+        <v>85</v>
+      </c>
+      <c r="S470">
+        <v>8</v>
+      </c>
+      <c r="T470">
+        <v>44.1</v>
+      </c>
+      <c r="U470">
+        <v>15</v>
+      </c>
+      <c r="V470">
+        <v>53.7</v>
+      </c>
+      <c r="W470">
+        <v>5</v>
+      </c>
+      <c r="X470">
+        <v>19.399999999999999</v>
+      </c>
+      <c r="Y470">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="471" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A471" t="s">
         <v>53</v>
       </c>
@@ -34638,8 +35037,83 @@
       <c r="D471" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="472" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E471">
+        <v>100</v>
+      </c>
+      <c r="F471">
+        <v>70.599999999999994</v>
+      </c>
+      <c r="G471">
+        <v>100</v>
+      </c>
+      <c r="H471">
+        <v>100</v>
+      </c>
+      <c r="I471">
+        <v>100</v>
+      </c>
+      <c r="J471">
+        <v>72.8</v>
+      </c>
+      <c r="K471">
+        <v>92</v>
+      </c>
+      <c r="L471">
+        <v>72.900000000000006</v>
+      </c>
+      <c r="M471">
+        <v>91</v>
+      </c>
+      <c r="N471">
+        <v>72.7</v>
+      </c>
+      <c r="O471">
+        <v>90</v>
+      </c>
+      <c r="P471">
+        <v>72.8</v>
+      </c>
+      <c r="Q471">
+        <v>65</v>
+      </c>
+      <c r="R471">
+        <v>73.2</v>
+      </c>
+      <c r="S471">
+        <v>59</v>
+      </c>
+      <c r="T471">
+        <v>42.4</v>
+      </c>
+      <c r="U471">
+        <v>8</v>
+      </c>
+      <c r="V471">
+        <v>44.1</v>
+      </c>
+      <c r="W471">
+        <v>7</v>
+      </c>
+      <c r="X471">
+        <v>44.8</v>
+      </c>
+      <c r="Y471">
+        <v>7</v>
+      </c>
+      <c r="Z471">
+        <v>48</v>
+      </c>
+      <c r="AA471">
+        <v>6</v>
+      </c>
+      <c r="AB471">
+        <v>48.6</v>
+      </c>
+      <c r="AC471">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="472" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A472" t="s">
         <v>53</v>
       </c>
@@ -34652,8 +35126,53 @@
       <c r="D472" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="473" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E472">
+        <v>100</v>
+      </c>
+      <c r="F472">
+        <v>72</v>
+      </c>
+      <c r="G472">
+        <v>80.2</v>
+      </c>
+      <c r="H472">
+        <v>100</v>
+      </c>
+      <c r="I472">
+        <v>100</v>
+      </c>
+      <c r="J472">
+        <v>72</v>
+      </c>
+      <c r="K472">
+        <v>99</v>
+      </c>
+      <c r="L472">
+        <v>76.099999999999994</v>
+      </c>
+      <c r="M472">
+        <v>56</v>
+      </c>
+      <c r="N472">
+        <v>81.900000000000006</v>
+      </c>
+      <c r="O472">
+        <v>9</v>
+      </c>
+      <c r="P472">
+        <v>81.2</v>
+      </c>
+      <c r="Q472">
+        <v>15</v>
+      </c>
+      <c r="R472">
+        <v>80.400000000000006</v>
+      </c>
+      <c r="S472">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="473" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A473" t="s">
         <v>53</v>
       </c>
@@ -34666,8 +35185,71 @@
       <c r="D473" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="474" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E473">
+        <v>100</v>
+      </c>
+      <c r="F473">
+        <v>71.599999999999994</v>
+      </c>
+      <c r="G473">
+        <v>99.2</v>
+      </c>
+      <c r="H473">
+        <v>100</v>
+      </c>
+      <c r="I473">
+        <v>100</v>
+      </c>
+      <c r="J473">
+        <v>82.5</v>
+      </c>
+      <c r="K473">
+        <v>5</v>
+      </c>
+      <c r="L473">
+        <v>77.900000000000006</v>
+      </c>
+      <c r="M473">
+        <v>52</v>
+      </c>
+      <c r="N473">
+        <v>77.900000000000006</v>
+      </c>
+      <c r="O473">
+        <v>12</v>
+      </c>
+      <c r="P473">
+        <v>80.599999999999994</v>
+      </c>
+      <c r="Q473">
+        <v>9</v>
+      </c>
+      <c r="R473">
+        <v>83</v>
+      </c>
+      <c r="S473">
+        <v>12</v>
+      </c>
+      <c r="T473">
+        <v>49</v>
+      </c>
+      <c r="U473">
+        <v>6</v>
+      </c>
+      <c r="V473">
+        <v>54.5</v>
+      </c>
+      <c r="W473">
+        <v>6</v>
+      </c>
+      <c r="X473">
+        <v>27</v>
+      </c>
+      <c r="Y473">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="474" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A474" t="s">
         <v>53</v>
       </c>
@@ -34680,8 +35262,83 @@
       <c r="D474" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="475" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E474">
+        <v>83.3</v>
+      </c>
+      <c r="F474">
+        <v>71.5</v>
+      </c>
+      <c r="G474">
+        <v>89.2</v>
+      </c>
+      <c r="H474">
+        <v>80.8</v>
+      </c>
+      <c r="I474">
+        <v>85.9</v>
+      </c>
+      <c r="J474">
+        <v>80</v>
+      </c>
+      <c r="K474">
+        <v>39</v>
+      </c>
+      <c r="L474">
+        <v>90.8</v>
+      </c>
+      <c r="M474">
+        <v>12</v>
+      </c>
+      <c r="N474">
+        <v>93.8</v>
+      </c>
+      <c r="O474">
+        <v>8</v>
+      </c>
+      <c r="P474">
+        <v>97.8</v>
+      </c>
+      <c r="Q474">
+        <v>6</v>
+      </c>
+      <c r="R474">
+        <v>95.3</v>
+      </c>
+      <c r="S474">
+        <v>5</v>
+      </c>
+      <c r="T474">
+        <v>39.700000000000003</v>
+      </c>
+      <c r="U474">
+        <v>15</v>
+      </c>
+      <c r="V474">
+        <v>48.9</v>
+      </c>
+      <c r="W474">
+        <v>6</v>
+      </c>
+      <c r="X474">
+        <v>51.1</v>
+      </c>
+      <c r="Y474">
+        <v>6</v>
+      </c>
+      <c r="Z474">
+        <v>46.3</v>
+      </c>
+      <c r="AA474">
+        <v>5</v>
+      </c>
+      <c r="AB474">
+        <v>37.6</v>
+      </c>
+      <c r="AC474">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="475" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A475" t="s">
         <v>53</v>
       </c>
@@ -34694,8 +35351,71 @@
       <c r="D475" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="476" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E475">
+        <v>98.2</v>
+      </c>
+      <c r="F475">
+        <v>64.099999999999994</v>
+      </c>
+      <c r="G475">
+        <v>42.2</v>
+      </c>
+      <c r="H475">
+        <v>98</v>
+      </c>
+      <c r="I475">
+        <v>98.6</v>
+      </c>
+      <c r="J475">
+        <v>77.8</v>
+      </c>
+      <c r="K475">
+        <v>46</v>
+      </c>
+      <c r="L475">
+        <v>86.4</v>
+      </c>
+      <c r="M475">
+        <v>24</v>
+      </c>
+      <c r="N475">
+        <v>90.1</v>
+      </c>
+      <c r="O475">
+        <v>17</v>
+      </c>
+      <c r="P475">
+        <v>88.5</v>
+      </c>
+      <c r="Q475">
+        <v>13</v>
+      </c>
+      <c r="R475">
+        <v>91.1</v>
+      </c>
+      <c r="S475">
+        <v>7</v>
+      </c>
+      <c r="T475">
+        <v>35.700000000000003</v>
+      </c>
+      <c r="U475">
+        <v>28</v>
+      </c>
+      <c r="V475">
+        <v>44.9</v>
+      </c>
+      <c r="W475">
+        <v>9</v>
+      </c>
+      <c r="X475">
+        <v>33.299999999999997</v>
+      </c>
+      <c r="Y475">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="476" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A476" t="s">
         <v>53</v>
       </c>
@@ -34708,8 +35428,77 @@
       <c r="D476" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="477" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E476">
+        <v>72.099999999999994</v>
+      </c>
+      <c r="F476">
+        <v>71.5</v>
+      </c>
+      <c r="G476">
+        <v>70.2</v>
+      </c>
+      <c r="H476">
+        <v>100</v>
+      </c>
+      <c r="I476">
+        <v>98.5</v>
+      </c>
+      <c r="J476">
+        <v>83.1</v>
+      </c>
+      <c r="K476">
+        <v>23</v>
+      </c>
+      <c r="L476">
+        <v>93.4</v>
+      </c>
+      <c r="M476">
+        <v>8</v>
+      </c>
+      <c r="N476">
+        <v>93.3</v>
+      </c>
+      <c r="O476">
+        <v>10</v>
+      </c>
+      <c r="P476">
+        <v>94.9</v>
+      </c>
+      <c r="Q476">
+        <v>5</v>
+      </c>
+      <c r="R476">
+        <v>92.9</v>
+      </c>
+      <c r="S476">
+        <v>5</v>
+      </c>
+      <c r="T476">
+        <v>37.799999999999997</v>
+      </c>
+      <c r="U476">
+        <v>21</v>
+      </c>
+      <c r="V476">
+        <v>43.5</v>
+      </c>
+      <c r="W476">
+        <v>6</v>
+      </c>
+      <c r="X476">
+        <v>31.3</v>
+      </c>
+      <c r="Y476">
+        <v>30</v>
+      </c>
+      <c r="Z476">
+        <v>26.6</v>
+      </c>
+      <c r="AA476">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="477" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A477" t="s">
         <v>53</v>
       </c>
@@ -34722,8 +35511,77 @@
       <c r="D477" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="478" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E477">
+        <v>85.3</v>
+      </c>
+      <c r="F477">
+        <v>70.599999999999994</v>
+      </c>
+      <c r="G477">
+        <v>81.7</v>
+      </c>
+      <c r="H477">
+        <v>93.1</v>
+      </c>
+      <c r="I477">
+        <v>82.4</v>
+      </c>
+      <c r="J477">
+        <v>74.099999999999994</v>
+      </c>
+      <c r="K477">
+        <v>76</v>
+      </c>
+      <c r="L477">
+        <v>78.3</v>
+      </c>
+      <c r="M477">
+        <v>33</v>
+      </c>
+      <c r="N477">
+        <v>83.3</v>
+      </c>
+      <c r="O477">
+        <v>13</v>
+      </c>
+      <c r="P477">
+        <v>90.7</v>
+      </c>
+      <c r="Q477">
+        <v>7</v>
+      </c>
+      <c r="R477">
+        <v>97.4</v>
+      </c>
+      <c r="S477">
+        <v>5</v>
+      </c>
+      <c r="T477">
+        <v>42.1</v>
+      </c>
+      <c r="U477">
+        <v>12</v>
+      </c>
+      <c r="V477">
+        <v>38.9</v>
+      </c>
+      <c r="W477">
+        <v>7</v>
+      </c>
+      <c r="X477">
+        <v>35.6</v>
+      </c>
+      <c r="Y477">
+        <v>6</v>
+      </c>
+      <c r="Z477">
+        <v>30.6</v>
+      </c>
+      <c r="AA477">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="478" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A478" t="s">
         <v>53</v>
       </c>
@@ -34736,8 +35594,53 @@
       <c r="D478" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="479" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E478">
+        <v>99.9</v>
+      </c>
+      <c r="F478">
+        <v>69.5</v>
+      </c>
+      <c r="G478">
+        <v>52.9</v>
+      </c>
+      <c r="H478">
+        <v>100</v>
+      </c>
+      <c r="I478">
+        <v>99.9</v>
+      </c>
+      <c r="J478">
+        <v>73.2</v>
+      </c>
+      <c r="K478">
+        <v>71</v>
+      </c>
+      <c r="L478">
+        <v>84.6</v>
+      </c>
+      <c r="M478">
+        <v>25</v>
+      </c>
+      <c r="N478">
+        <v>88.3</v>
+      </c>
+      <c r="O478">
+        <v>21</v>
+      </c>
+      <c r="P478">
+        <v>87.3</v>
+      </c>
+      <c r="Q478">
+        <v>8</v>
+      </c>
+      <c r="T478">
+        <v>40.4</v>
+      </c>
+      <c r="U478">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="479" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A479" t="s">
         <v>53</v>
       </c>
@@ -34750,8 +35653,71 @@
       <c r="D479" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="480" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E479">
+        <v>99.3</v>
+      </c>
+      <c r="F479">
+        <v>71.5</v>
+      </c>
+      <c r="G479">
+        <v>76.400000000000006</v>
+      </c>
+      <c r="H479">
+        <v>100</v>
+      </c>
+      <c r="I479">
+        <v>99.5</v>
+      </c>
+      <c r="J479">
+        <v>80.900000000000006</v>
+      </c>
+      <c r="K479">
+        <v>30</v>
+      </c>
+      <c r="L479">
+        <v>92.1</v>
+      </c>
+      <c r="M479">
+        <v>5</v>
+      </c>
+      <c r="N479">
+        <v>87.9</v>
+      </c>
+      <c r="O479">
+        <v>7</v>
+      </c>
+      <c r="P479">
+        <v>92.5</v>
+      </c>
+      <c r="Q479">
+        <v>5</v>
+      </c>
+      <c r="R479">
+        <v>92.3</v>
+      </c>
+      <c r="S479">
+        <v>5</v>
+      </c>
+      <c r="T479">
+        <v>43.2</v>
+      </c>
+      <c r="U479">
+        <v>5</v>
+      </c>
+      <c r="V479">
+        <v>35.5</v>
+      </c>
+      <c r="W479">
+        <v>14</v>
+      </c>
+      <c r="X479">
+        <v>32.700000000000003</v>
+      </c>
+      <c r="Y479">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="480" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A480" t="s">
         <v>53</v>
       </c>
@@ -34764,8 +35730,83 @@
       <c r="D480" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="481" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E480">
+        <v>92</v>
+      </c>
+      <c r="F480">
+        <v>70.5</v>
+      </c>
+      <c r="G480">
+        <v>89.6</v>
+      </c>
+      <c r="H480">
+        <v>94.1</v>
+      </c>
+      <c r="I480">
+        <v>91.4</v>
+      </c>
+      <c r="J480">
+        <v>74.2</v>
+      </c>
+      <c r="K480">
+        <v>65</v>
+      </c>
+      <c r="L480">
+        <v>75.599999999999994</v>
+      </c>
+      <c r="M480">
+        <v>45</v>
+      </c>
+      <c r="N480">
+        <v>80.8</v>
+      </c>
+      <c r="O480">
+        <v>19</v>
+      </c>
+      <c r="P480">
+        <v>89.5</v>
+      </c>
+      <c r="Q480">
+        <v>5</v>
+      </c>
+      <c r="R480">
+        <v>90.4</v>
+      </c>
+      <c r="S480">
+        <v>11</v>
+      </c>
+      <c r="T480">
+        <v>42.9</v>
+      </c>
+      <c r="U480">
+        <v>8</v>
+      </c>
+      <c r="V480">
+        <v>51.2</v>
+      </c>
+      <c r="W480">
+        <v>5</v>
+      </c>
+      <c r="X480">
+        <v>48.9</v>
+      </c>
+      <c r="Y480">
+        <v>6</v>
+      </c>
+      <c r="Z480">
+        <v>54.1</v>
+      </c>
+      <c r="AA480">
+        <v>5</v>
+      </c>
+      <c r="AB480">
+        <v>50</v>
+      </c>
+      <c r="AC480">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="481" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A481" t="s">
         <v>53</v>
       </c>
@@ -34778,8 +35819,53 @@
       <c r="D481" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="482" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E481">
+        <v>100</v>
+      </c>
+      <c r="F481">
+        <v>71.400000000000006</v>
+      </c>
+      <c r="G481">
+        <v>45.8</v>
+      </c>
+      <c r="H481">
+        <v>100</v>
+      </c>
+      <c r="I481">
+        <v>100</v>
+      </c>
+      <c r="J481">
+        <v>73.400000000000006</v>
+      </c>
+      <c r="K481">
+        <v>74</v>
+      </c>
+      <c r="L481">
+        <v>84.2</v>
+      </c>
+      <c r="M481">
+        <v>26</v>
+      </c>
+      <c r="N481">
+        <v>88.5</v>
+      </c>
+      <c r="O481">
+        <v>20</v>
+      </c>
+      <c r="P481">
+        <v>89.3</v>
+      </c>
+      <c r="Q481">
+        <v>10</v>
+      </c>
+      <c r="T481">
+        <v>46.8</v>
+      </c>
+      <c r="U481">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="482" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A482" t="s">
         <v>53</v>
       </c>
@@ -34792,8 +35878,77 @@
       <c r="D482" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="483" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E482">
+        <v>100</v>
+      </c>
+      <c r="F482">
+        <v>71.599999999999994</v>
+      </c>
+      <c r="G482">
+        <v>84.5</v>
+      </c>
+      <c r="H482">
+        <v>100</v>
+      </c>
+      <c r="I482">
+        <v>100</v>
+      </c>
+      <c r="J482">
+        <v>74.900000000000006</v>
+      </c>
+      <c r="K482">
+        <v>37</v>
+      </c>
+      <c r="L482">
+        <v>84.4</v>
+      </c>
+      <c r="M482">
+        <v>11</v>
+      </c>
+      <c r="N482">
+        <v>87.9</v>
+      </c>
+      <c r="O482">
+        <v>8</v>
+      </c>
+      <c r="P482">
+        <v>86.1</v>
+      </c>
+      <c r="Q482">
+        <v>24</v>
+      </c>
+      <c r="R482">
+        <v>93.5</v>
+      </c>
+      <c r="S482">
+        <v>6</v>
+      </c>
+      <c r="T482">
+        <v>49</v>
+      </c>
+      <c r="U482">
+        <v>6</v>
+      </c>
+      <c r="V482">
+        <v>46.3</v>
+      </c>
+      <c r="W482">
+        <v>5</v>
+      </c>
+      <c r="X482">
+        <v>48.6</v>
+      </c>
+      <c r="Y482">
+        <v>5</v>
+      </c>
+      <c r="Z482">
+        <v>37.799999999999997</v>
+      </c>
+      <c r="AA482">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="483" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A483" t="s">
         <v>53</v>
       </c>
@@ -34807,7 +35962,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="484" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="484" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A484" t="s">
         <v>53</v>
       </c>
@@ -34820,8 +35975,65 @@
       <c r="D484" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="485" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E484">
+        <v>97.4</v>
+      </c>
+      <c r="F484">
+        <v>62.5</v>
+      </c>
+      <c r="G484">
+        <v>42.5</v>
+      </c>
+      <c r="H484">
+        <v>97.8</v>
+      </c>
+      <c r="I484">
+        <v>97.1</v>
+      </c>
+      <c r="J484">
+        <v>80.599999999999994</v>
+      </c>
+      <c r="K484">
+        <v>51</v>
+      </c>
+      <c r="L484">
+        <v>87.5</v>
+      </c>
+      <c r="M484">
+        <v>28</v>
+      </c>
+      <c r="N484">
+        <v>89.3</v>
+      </c>
+      <c r="O484">
+        <v>17</v>
+      </c>
+      <c r="P484">
+        <v>97.4</v>
+      </c>
+      <c r="Q484">
+        <v>5</v>
+      </c>
+      <c r="T484">
+        <v>39.200000000000003</v>
+      </c>
+      <c r="U484">
+        <v>42</v>
+      </c>
+      <c r="V484">
+        <v>44.7</v>
+      </c>
+      <c r="W484">
+        <v>23</v>
+      </c>
+      <c r="X484">
+        <v>53.7</v>
+      </c>
+      <c r="Y484">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="485" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A485" t="s">
         <v>53</v>
       </c>
@@ -34834,8 +36046,71 @@
       <c r="D485" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="486" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E485">
+        <v>74</v>
+      </c>
+      <c r="F485">
+        <v>71</v>
+      </c>
+      <c r="G485">
+        <v>24.5</v>
+      </c>
+      <c r="H485">
+        <v>99.5</v>
+      </c>
+      <c r="I485">
+        <v>99.1</v>
+      </c>
+      <c r="J485">
+        <v>89.2</v>
+      </c>
+      <c r="K485">
+        <v>5</v>
+      </c>
+      <c r="L485">
+        <v>86.8</v>
+      </c>
+      <c r="M485">
+        <v>13</v>
+      </c>
+      <c r="N485">
+        <v>97.4</v>
+      </c>
+      <c r="O485">
+        <v>5</v>
+      </c>
+      <c r="P485">
+        <v>89.2</v>
+      </c>
+      <c r="Q485">
+        <v>8</v>
+      </c>
+      <c r="R485">
+        <v>86.8</v>
+      </c>
+      <c r="S485">
+        <v>5</v>
+      </c>
+      <c r="T485">
+        <v>36.700000000000003</v>
+      </c>
+      <c r="U485">
+        <v>49</v>
+      </c>
+      <c r="V485">
+        <v>40.5</v>
+      </c>
+      <c r="W485">
+        <v>20</v>
+      </c>
+      <c r="X485">
+        <v>51.1</v>
+      </c>
+      <c r="Y485">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="486" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A486" t="s">
         <v>53</v>
       </c>
@@ -34848,8 +36123,83 @@
       <c r="D486" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="487" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E486">
+        <v>99.9</v>
+      </c>
+      <c r="F486">
+        <v>69.5</v>
+      </c>
+      <c r="G486">
+        <v>97.2</v>
+      </c>
+      <c r="H486">
+        <v>99.8</v>
+      </c>
+      <c r="I486">
+        <v>99.9</v>
+      </c>
+      <c r="J486">
+        <v>76.900000000000006</v>
+      </c>
+      <c r="K486">
+        <v>63</v>
+      </c>
+      <c r="L486">
+        <v>77.2</v>
+      </c>
+      <c r="M486">
+        <v>62</v>
+      </c>
+      <c r="N486">
+        <v>78</v>
+      </c>
+      <c r="O486">
+        <v>47</v>
+      </c>
+      <c r="P486">
+        <v>80.3</v>
+      </c>
+      <c r="Q486">
+        <v>30</v>
+      </c>
+      <c r="R486">
+        <v>82.7</v>
+      </c>
+      <c r="S486">
+        <v>10</v>
+      </c>
+      <c r="T486">
+        <v>38.4</v>
+      </c>
+      <c r="U486">
+        <v>9</v>
+      </c>
+      <c r="V486">
+        <v>37.200000000000003</v>
+      </c>
+      <c r="W486">
+        <v>37</v>
+      </c>
+      <c r="X486">
+        <v>42.6</v>
+      </c>
+      <c r="Y486">
+        <v>7</v>
+      </c>
+      <c r="Z486">
+        <v>41.2</v>
+      </c>
+      <c r="AA486">
+        <v>13</v>
+      </c>
+      <c r="AB486">
+        <v>52.4</v>
+      </c>
+      <c r="AC486">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="487" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A487" t="s">
         <v>53</v>
       </c>
@@ -34862,8 +36212,65 @@
       <c r="D487" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="488" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E487">
+        <v>100</v>
+      </c>
+      <c r="F487">
+        <v>59.8</v>
+      </c>
+      <c r="G487">
+        <v>35.700000000000003</v>
+      </c>
+      <c r="H487">
+        <v>100</v>
+      </c>
+      <c r="I487">
+        <v>100</v>
+      </c>
+      <c r="J487">
+        <v>76.400000000000006</v>
+      </c>
+      <c r="K487">
+        <v>49</v>
+      </c>
+      <c r="L487">
+        <v>85.3</v>
+      </c>
+      <c r="M487">
+        <v>27</v>
+      </c>
+      <c r="N487">
+        <v>89.6</v>
+      </c>
+      <c r="O487">
+        <v>16</v>
+      </c>
+      <c r="P487">
+        <v>91.7</v>
+      </c>
+      <c r="Q487">
+        <v>8</v>
+      </c>
+      <c r="T487">
+        <v>33.6</v>
+      </c>
+      <c r="U487">
+        <v>36</v>
+      </c>
+      <c r="V487">
+        <v>40.1</v>
+      </c>
+      <c r="W487">
+        <v>22</v>
+      </c>
+      <c r="X487">
+        <v>40.4</v>
+      </c>
+      <c r="Y487">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="488" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A488" t="s">
         <v>53</v>
       </c>
@@ -34876,8 +36283,83 @@
       <c r="D488" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="489" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E488">
+        <v>100</v>
+      </c>
+      <c r="F488">
+        <v>71.5</v>
+      </c>
+      <c r="G488">
+        <v>83.5</v>
+      </c>
+      <c r="H488">
+        <v>100</v>
+      </c>
+      <c r="I488">
+        <v>100</v>
+      </c>
+      <c r="J488">
+        <v>76.099999999999994</v>
+      </c>
+      <c r="K488">
+        <v>56</v>
+      </c>
+      <c r="L488">
+        <v>77</v>
+      </c>
+      <c r="M488">
+        <v>47</v>
+      </c>
+      <c r="N488">
+        <v>91.8</v>
+      </c>
+      <c r="O488">
+        <v>6</v>
+      </c>
+      <c r="P488">
+        <v>86.1</v>
+      </c>
+      <c r="Q488">
+        <v>5</v>
+      </c>
+      <c r="R488">
+        <v>80.599999999999994</v>
+      </c>
+      <c r="S488">
+        <v>13</v>
+      </c>
+      <c r="T488">
+        <v>37.700000000000003</v>
+      </c>
+      <c r="U488">
+        <v>14</v>
+      </c>
+      <c r="V488">
+        <v>41.3</v>
+      </c>
+      <c r="W488">
+        <v>6</v>
+      </c>
+      <c r="X488">
+        <v>40.5</v>
+      </c>
+      <c r="Y488">
+        <v>5</v>
+      </c>
+      <c r="Z488">
+        <v>41.3</v>
+      </c>
+      <c r="AA488">
+        <v>8</v>
+      </c>
+      <c r="AB488">
+        <v>37.799999999999997</v>
+      </c>
+      <c r="AC488">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="489" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A489" t="s">
         <v>53</v>
       </c>
@@ -34890,8 +36372,83 @@
       <c r="D489" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="490" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E489">
+        <v>100</v>
+      </c>
+      <c r="F489">
+        <v>62.9</v>
+      </c>
+      <c r="G489">
+        <v>99.6</v>
+      </c>
+      <c r="H489">
+        <v>100</v>
+      </c>
+      <c r="I489">
+        <v>100</v>
+      </c>
+      <c r="J489">
+        <v>90.5</v>
+      </c>
+      <c r="K489">
+        <v>12</v>
+      </c>
+      <c r="L489">
+        <v>92.9</v>
+      </c>
+      <c r="M489">
+        <v>5</v>
+      </c>
+      <c r="N489">
+        <v>90.9</v>
+      </c>
+      <c r="O489">
+        <v>6</v>
+      </c>
+      <c r="P489">
+        <v>91.7</v>
+      </c>
+      <c r="Q489">
+        <v>5</v>
+      </c>
+      <c r="R489">
+        <v>93.3</v>
+      </c>
+      <c r="S489">
+        <v>6</v>
+      </c>
+      <c r="T489">
+        <v>32.4</v>
+      </c>
+      <c r="U489">
+        <v>48</v>
+      </c>
+      <c r="V489">
+        <v>33.5</v>
+      </c>
+      <c r="W489">
+        <v>44</v>
+      </c>
+      <c r="X489">
+        <v>33.700000000000003</v>
+      </c>
+      <c r="Y489">
+        <v>40</v>
+      </c>
+      <c r="Z489">
+        <v>39</v>
+      </c>
+      <c r="AA489">
+        <v>21</v>
+      </c>
+      <c r="AB489">
+        <v>38.299999999999997</v>
+      </c>
+      <c r="AC489">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="490" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A490" t="s">
         <v>53</v>
       </c>
@@ -34904,8 +36461,65 @@
       <c r="D490" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="491" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E490">
+        <v>100</v>
+      </c>
+      <c r="F490">
+        <v>60.7</v>
+      </c>
+      <c r="G490">
+        <v>31.8</v>
+      </c>
+      <c r="H490">
+        <v>100</v>
+      </c>
+      <c r="I490">
+        <v>100</v>
+      </c>
+      <c r="J490">
+        <v>83.1</v>
+      </c>
+      <c r="K490">
+        <v>34</v>
+      </c>
+      <c r="L490">
+        <v>85.9</v>
+      </c>
+      <c r="M490">
+        <v>23</v>
+      </c>
+      <c r="N490">
+        <v>88.9</v>
+      </c>
+      <c r="O490">
+        <v>16</v>
+      </c>
+      <c r="P490">
+        <v>95.1</v>
+      </c>
+      <c r="Q490">
+        <v>5</v>
+      </c>
+      <c r="T490">
+        <v>36.700000000000003</v>
+      </c>
+      <c r="U490">
+        <v>41</v>
+      </c>
+      <c r="V490">
+        <v>40.1</v>
+      </c>
+      <c r="W490">
+        <v>19</v>
+      </c>
+      <c r="X490">
+        <v>40.700000000000003</v>
+      </c>
+      <c r="Y490">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="491" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A491" t="s">
         <v>53</v>
       </c>
@@ -34918,10 +36532,85 @@
       <c r="D491" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="492" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E491">
+        <v>100</v>
+      </c>
+      <c r="F491">
+        <v>71.5</v>
+      </c>
+      <c r="G491">
+        <v>98.4</v>
+      </c>
+      <c r="H491">
+        <v>100</v>
+      </c>
+      <c r="I491">
+        <v>100</v>
+      </c>
+      <c r="J491">
+        <v>97.8</v>
+      </c>
+      <c r="K491">
+        <v>6</v>
+      </c>
+      <c r="L491">
+        <v>97.6</v>
+      </c>
+      <c r="M491">
+        <v>5</v>
+      </c>
+      <c r="N491">
+        <v>97.4</v>
+      </c>
+      <c r="O491">
+        <v>5</v>
+      </c>
+      <c r="P491">
+        <v>97.3</v>
+      </c>
+      <c r="Q491">
+        <v>5</v>
+      </c>
+      <c r="R491">
+        <v>97.4</v>
+      </c>
+      <c r="S491">
+        <v>5</v>
+      </c>
+      <c r="T491">
+        <v>34.5</v>
+      </c>
+      <c r="U491">
+        <v>56</v>
+      </c>
+      <c r="V491">
+        <v>36.4</v>
+      </c>
+      <c r="W491">
+        <v>8</v>
+      </c>
+      <c r="X491">
+        <v>36.9</v>
+      </c>
+      <c r="Y491">
+        <v>32</v>
+      </c>
+      <c r="Z491">
+        <v>39.5</v>
+      </c>
+      <c r="AA491">
+        <v>16</v>
+      </c>
+      <c r="AB491">
+        <v>40.4</v>
+      </c>
+      <c r="AC491">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="492" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A492" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B492" t="s">
         <v>25</v>
@@ -34929,10 +36618,85 @@
       <c r="D492" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="493" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E492">
+        <v>100</v>
+      </c>
+      <c r="F492">
+        <v>60.6</v>
+      </c>
+      <c r="G492">
+        <v>100</v>
+      </c>
+      <c r="H492">
+        <v>100</v>
+      </c>
+      <c r="I492">
+        <v>100</v>
+      </c>
+      <c r="J492">
+        <v>95</v>
+      </c>
+      <c r="K492">
+        <v>5</v>
+      </c>
+      <c r="L492">
+        <v>96.6</v>
+      </c>
+      <c r="M492">
+        <v>7</v>
+      </c>
+      <c r="N492">
+        <v>100</v>
+      </c>
+      <c r="O492">
+        <v>6</v>
+      </c>
+      <c r="P492">
+        <v>97.4</v>
+      </c>
+      <c r="Q492">
+        <v>5</v>
+      </c>
+      <c r="R492">
+        <v>97.4</v>
+      </c>
+      <c r="S492">
+        <v>5</v>
+      </c>
+      <c r="T492">
+        <v>33.299999999999997</v>
+      </c>
+      <c r="U492">
+        <v>33</v>
+      </c>
+      <c r="V492">
+        <v>33</v>
+      </c>
+      <c r="W492">
+        <v>49</v>
+      </c>
+      <c r="X492">
+        <v>33.200000000000003</v>
+      </c>
+      <c r="Y492">
+        <v>52</v>
+      </c>
+      <c r="Z492">
+        <v>33.299999999999997</v>
+      </c>
+      <c r="AA492">
+        <v>50</v>
+      </c>
+      <c r="AB492">
+        <v>34.1</v>
+      </c>
+      <c r="AC492">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="493" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A493" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B493" t="s">
         <v>25</v>
@@ -34940,16 +36704,2257 @@
       <c r="D493" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="494" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E493">
+        <v>100</v>
+      </c>
+      <c r="F493">
+        <v>62</v>
+      </c>
+      <c r="G493">
+        <v>11.3</v>
+      </c>
+      <c r="H493">
+        <v>100</v>
+      </c>
+      <c r="I493">
+        <v>100</v>
+      </c>
+      <c r="J493">
+        <v>82.8</v>
+      </c>
+      <c r="K493">
+        <v>41</v>
+      </c>
+      <c r="L493">
+        <v>94.6</v>
+      </c>
+      <c r="M493">
+        <v>5</v>
+      </c>
+      <c r="N493">
+        <v>92.5</v>
+      </c>
+      <c r="O493">
+        <v>7</v>
+      </c>
+      <c r="T493">
+        <v>36.9</v>
+      </c>
+      <c r="U493">
+        <v>54</v>
+      </c>
+      <c r="V493">
+        <v>45.8</v>
+      </c>
+      <c r="W493">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="494" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A494" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B494" t="s">
         <v>25</v>
       </c>
       <c r="D494" t="s">
         <v>30</v>
+      </c>
+      <c r="E494">
+        <v>100</v>
+      </c>
+      <c r="F494">
+        <v>72.099999999999994</v>
+      </c>
+      <c r="G494">
+        <v>96.1</v>
+      </c>
+      <c r="H494">
+        <v>100</v>
+      </c>
+      <c r="I494">
+        <v>100</v>
+      </c>
+      <c r="J494">
+        <v>87.2</v>
+      </c>
+      <c r="K494">
+        <v>5</v>
+      </c>
+      <c r="L494">
+        <v>86.3</v>
+      </c>
+      <c r="M494">
+        <v>6</v>
+      </c>
+      <c r="N494">
+        <v>87.5</v>
+      </c>
+      <c r="O494">
+        <v>5</v>
+      </c>
+      <c r="P494">
+        <v>86.8</v>
+      </c>
+      <c r="Q494">
+        <v>5</v>
+      </c>
+      <c r="R494">
+        <v>71.400000000000006</v>
+      </c>
+      <c r="S494">
+        <v>5</v>
+      </c>
+      <c r="T494">
+        <v>48.8</v>
+      </c>
+      <c r="U494">
+        <v>5</v>
+      </c>
+      <c r="V494">
+        <v>46.8</v>
+      </c>
+      <c r="W494">
+        <v>8</v>
+      </c>
+      <c r="X494">
+        <v>55.8</v>
+      </c>
+      <c r="Y494">
+        <v>5</v>
+      </c>
+      <c r="Z494">
+        <v>51.8</v>
+      </c>
+      <c r="AA494">
+        <v>7</v>
+      </c>
+      <c r="AB494">
+        <v>38.6</v>
+      </c>
+      <c r="AC494">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="495" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A495" t="s">
+        <v>54</v>
+      </c>
+      <c r="B495" t="s">
+        <v>28</v>
+      </c>
+      <c r="C495">
+        <v>5</v>
+      </c>
+      <c r="D495" t="s">
+        <v>26</v>
+      </c>
+      <c r="E495">
+        <v>95.4</v>
+      </c>
+      <c r="F495">
+        <v>63.5</v>
+      </c>
+      <c r="G495">
+        <v>96.8</v>
+      </c>
+      <c r="H495">
+        <v>95.3</v>
+      </c>
+      <c r="I495">
+        <v>95.6</v>
+      </c>
+      <c r="J495">
+        <v>84.2</v>
+      </c>
+      <c r="K495">
+        <v>21</v>
+      </c>
+      <c r="L495">
+        <v>94.6</v>
+      </c>
+      <c r="M495">
+        <v>5</v>
+      </c>
+      <c r="N495">
+        <v>87.3</v>
+      </c>
+      <c r="O495">
+        <v>8</v>
+      </c>
+      <c r="P495">
+        <v>88.9</v>
+      </c>
+      <c r="Q495">
+        <v>6</v>
+      </c>
+      <c r="R495">
+        <v>86.6</v>
+      </c>
+      <c r="S495">
+        <v>8</v>
+      </c>
+      <c r="T495">
+        <v>35.6</v>
+      </c>
+      <c r="U495">
+        <v>28</v>
+      </c>
+      <c r="V495">
+        <v>37</v>
+      </c>
+      <c r="W495">
+        <v>6</v>
+      </c>
+      <c r="X495">
+        <v>37.1</v>
+      </c>
+      <c r="Y495">
+        <v>9</v>
+      </c>
+      <c r="Z495">
+        <v>35.700000000000003</v>
+      </c>
+      <c r="AA495">
+        <v>16</v>
+      </c>
+      <c r="AB495">
+        <v>44.7</v>
+      </c>
+      <c r="AC495">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="496" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A496" t="s">
+        <v>54</v>
+      </c>
+      <c r="B496" t="s">
+        <v>28</v>
+      </c>
+      <c r="C496">
+        <v>5</v>
+      </c>
+      <c r="D496" t="s">
+        <v>29</v>
+      </c>
+      <c r="E496">
+        <v>100</v>
+      </c>
+      <c r="F496">
+        <v>68.099999999999994</v>
+      </c>
+      <c r="G496">
+        <v>30.2</v>
+      </c>
+      <c r="H496">
+        <v>100</v>
+      </c>
+      <c r="I496">
+        <v>100</v>
+      </c>
+      <c r="J496">
+        <v>72.099999999999994</v>
+      </c>
+      <c r="K496">
+        <v>51</v>
+      </c>
+      <c r="L496">
+        <v>72.8</v>
+      </c>
+      <c r="M496">
+        <v>28</v>
+      </c>
+      <c r="N496">
+        <v>81.2</v>
+      </c>
+      <c r="O496">
+        <v>13</v>
+      </c>
+      <c r="T496">
+        <v>29.2</v>
+      </c>
+      <c r="U496">
+        <v>49</v>
+      </c>
+      <c r="V496">
+        <v>25.3</v>
+      </c>
+      <c r="W496">
+        <v>31</v>
+      </c>
+      <c r="X496">
+        <v>14.7</v>
+      </c>
+      <c r="Y496">
+        <v>16</v>
+      </c>
+      <c r="Z496">
+        <v>12.5</v>
+      </c>
+      <c r="AA496">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="497" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A497" t="s">
+        <v>54</v>
+      </c>
+      <c r="B497" t="s">
+        <v>28</v>
+      </c>
+      <c r="C497">
+        <v>5</v>
+      </c>
+      <c r="D497" t="s">
+        <v>30</v>
+      </c>
+      <c r="E497">
+        <v>90.6</v>
+      </c>
+      <c r="F497">
+        <v>71.5</v>
+      </c>
+      <c r="G497">
+        <v>63.9</v>
+      </c>
+      <c r="H497">
+        <v>100</v>
+      </c>
+      <c r="I497">
+        <v>100</v>
+      </c>
+      <c r="J497">
+        <v>86</v>
+      </c>
+      <c r="K497">
+        <v>6</v>
+      </c>
+      <c r="L497">
+        <v>86.9</v>
+      </c>
+      <c r="M497">
+        <v>8</v>
+      </c>
+      <c r="N497">
+        <v>69.7</v>
+      </c>
+      <c r="O497">
+        <v>8</v>
+      </c>
+      <c r="P497">
+        <v>72.2</v>
+      </c>
+      <c r="Q497">
+        <v>14</v>
+      </c>
+      <c r="R497">
+        <v>65.099999999999994</v>
+      </c>
+      <c r="S497">
+        <v>19</v>
+      </c>
+      <c r="T497">
+        <v>36.700000000000003</v>
+      </c>
+      <c r="U497">
+        <v>28</v>
+      </c>
+      <c r="V497">
+        <v>38</v>
+      </c>
+      <c r="W497">
+        <v>14</v>
+      </c>
+      <c r="X497">
+        <v>41.4</v>
+      </c>
+      <c r="Y497">
+        <v>9</v>
+      </c>
+      <c r="Z497">
+        <v>34.200000000000003</v>
+      </c>
+      <c r="AA497">
+        <v>9</v>
+      </c>
+      <c r="AB497">
+        <v>36.200000000000003</v>
+      </c>
+      <c r="AC497">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="498" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A498" t="s">
+        <v>54</v>
+      </c>
+      <c r="B498" t="s">
+        <v>28</v>
+      </c>
+      <c r="C498">
+        <v>15</v>
+      </c>
+      <c r="D498" t="s">
+        <v>26</v>
+      </c>
+      <c r="E498">
+        <v>100</v>
+      </c>
+      <c r="F498">
+        <v>70.3</v>
+      </c>
+      <c r="G498">
+        <v>99.9</v>
+      </c>
+      <c r="H498">
+        <v>100</v>
+      </c>
+      <c r="I498">
+        <v>100</v>
+      </c>
+      <c r="J498">
+        <v>74.5</v>
+      </c>
+      <c r="K498">
+        <v>63</v>
+      </c>
+      <c r="L498">
+        <v>74.3</v>
+      </c>
+      <c r="M498">
+        <v>50</v>
+      </c>
+      <c r="N498">
+        <v>74.7</v>
+      </c>
+      <c r="O498">
+        <v>48</v>
+      </c>
+      <c r="P498">
+        <v>74.5</v>
+      </c>
+      <c r="Q498">
+        <v>46</v>
+      </c>
+      <c r="R498">
+        <v>78.400000000000006</v>
+      </c>
+      <c r="S498">
+        <v>29</v>
+      </c>
+      <c r="T498">
+        <v>42.1</v>
+      </c>
+      <c r="U498">
+        <v>7</v>
+      </c>
+      <c r="V498">
+        <v>45.7</v>
+      </c>
+      <c r="W498">
+        <v>6</v>
+      </c>
+      <c r="X498">
+        <v>40</v>
+      </c>
+      <c r="Y498">
+        <v>6</v>
+      </c>
+      <c r="Z498">
+        <v>38.1</v>
+      </c>
+      <c r="AA498">
+        <v>5</v>
+      </c>
+      <c r="AB498">
+        <v>35.1</v>
+      </c>
+      <c r="AC498">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="499" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A499" t="s">
+        <v>54</v>
+      </c>
+      <c r="B499" t="s">
+        <v>28</v>
+      </c>
+      <c r="C499">
+        <v>15</v>
+      </c>
+      <c r="D499" t="s">
+        <v>29</v>
+      </c>
+      <c r="E499">
+        <v>100</v>
+      </c>
+      <c r="F499">
+        <v>70.099999999999994</v>
+      </c>
+      <c r="G499">
+        <v>64.099999999999994</v>
+      </c>
+      <c r="H499">
+        <v>100</v>
+      </c>
+      <c r="I499">
+        <v>100</v>
+      </c>
+      <c r="J499">
+        <v>71.7</v>
+      </c>
+      <c r="K499">
+        <v>95</v>
+      </c>
+      <c r="L499">
+        <v>72.2</v>
+      </c>
+      <c r="M499">
+        <v>83</v>
+      </c>
+      <c r="N499">
+        <v>77.099999999999994</v>
+      </c>
+      <c r="O499">
+        <v>20</v>
+      </c>
+      <c r="P499">
+        <v>76.8</v>
+      </c>
+      <c r="Q499">
+        <v>9</v>
+      </c>
+      <c r="T499">
+        <v>33.299999999999997</v>
+      </c>
+      <c r="U499">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="500" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A500" t="s">
+        <v>54</v>
+      </c>
+      <c r="B500" t="s">
+        <v>28</v>
+      </c>
+      <c r="C500">
+        <v>15</v>
+      </c>
+      <c r="D500" t="s">
+        <v>30</v>
+      </c>
+      <c r="E500">
+        <v>100</v>
+      </c>
+      <c r="F500">
+        <v>71.5</v>
+      </c>
+      <c r="G500">
+        <v>82</v>
+      </c>
+      <c r="H500">
+        <v>100</v>
+      </c>
+      <c r="I500">
+        <v>100</v>
+      </c>
+      <c r="J500">
+        <v>82.5</v>
+      </c>
+      <c r="K500">
+        <v>10</v>
+      </c>
+      <c r="L500">
+        <v>75.5</v>
+      </c>
+      <c r="M500">
+        <v>30</v>
+      </c>
+      <c r="N500">
+        <v>93.3</v>
+      </c>
+      <c r="O500">
+        <v>8</v>
+      </c>
+      <c r="P500">
+        <v>75.599999999999994</v>
+      </c>
+      <c r="Q500">
+        <v>48</v>
+      </c>
+      <c r="R500">
+        <v>79.3</v>
+      </c>
+      <c r="S500">
+        <v>7</v>
+      </c>
+      <c r="T500">
+        <v>42.9</v>
+      </c>
+      <c r="U500">
+        <v>8</v>
+      </c>
+      <c r="V500">
+        <v>43.3</v>
+      </c>
+      <c r="W500">
+        <v>8</v>
+      </c>
+      <c r="X500">
+        <v>46.7</v>
+      </c>
+      <c r="Y500">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="501" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A501" t="s">
+        <v>54</v>
+      </c>
+      <c r="B501" t="s">
+        <v>28</v>
+      </c>
+      <c r="C501">
+        <v>25</v>
+      </c>
+      <c r="D501" t="s">
+        <v>26</v>
+      </c>
+      <c r="E501">
+        <v>100</v>
+      </c>
+      <c r="F501">
+        <v>70.5</v>
+      </c>
+      <c r="G501">
+        <v>99.7</v>
+      </c>
+      <c r="H501">
+        <v>100</v>
+      </c>
+      <c r="I501">
+        <v>100</v>
+      </c>
+      <c r="J501">
+        <v>74.900000000000006</v>
+      </c>
+      <c r="K501">
+        <v>72</v>
+      </c>
+      <c r="L501">
+        <v>74.8</v>
+      </c>
+      <c r="M501">
+        <v>72</v>
+      </c>
+      <c r="N501">
+        <v>75</v>
+      </c>
+      <c r="O501">
+        <v>71</v>
+      </c>
+      <c r="P501">
+        <v>75</v>
+      </c>
+      <c r="Q501">
+        <v>71</v>
+      </c>
+      <c r="R501">
+        <v>75.099999999999994</v>
+      </c>
+      <c r="S501">
+        <v>59</v>
+      </c>
+      <c r="T501">
+        <v>43.9</v>
+      </c>
+      <c r="U501">
+        <v>8</v>
+      </c>
+      <c r="V501">
+        <v>45</v>
+      </c>
+      <c r="W501">
+        <v>8</v>
+      </c>
+      <c r="X501">
+        <v>48.1</v>
+      </c>
+      <c r="Y501">
+        <v>7</v>
+      </c>
+      <c r="Z501">
+        <v>51.1</v>
+      </c>
+      <c r="AA501">
+        <v>6</v>
+      </c>
+      <c r="AB501">
+        <v>54.5</v>
+      </c>
+      <c r="AC501">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="502" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A502" t="s">
+        <v>54</v>
+      </c>
+      <c r="B502" t="s">
+        <v>28</v>
+      </c>
+      <c r="C502">
+        <v>25</v>
+      </c>
+      <c r="D502" t="s">
+        <v>29</v>
+      </c>
+      <c r="E502">
+        <v>100</v>
+      </c>
+      <c r="F502">
+        <v>70</v>
+      </c>
+      <c r="G502">
+        <v>48.2</v>
+      </c>
+      <c r="H502">
+        <v>100</v>
+      </c>
+      <c r="I502">
+        <v>100</v>
+      </c>
+      <c r="J502">
+        <v>71.5</v>
+      </c>
+      <c r="K502">
+        <v>95</v>
+      </c>
+      <c r="L502">
+        <v>77.3</v>
+      </c>
+      <c r="M502">
+        <v>42</v>
+      </c>
+      <c r="N502">
+        <v>91.3</v>
+      </c>
+      <c r="O502">
+        <v>6</v>
+      </c>
+      <c r="T502">
+        <v>28.9</v>
+      </c>
+      <c r="U502">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="503" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A503" t="s">
+        <v>54</v>
+      </c>
+      <c r="B503" t="s">
+        <v>28</v>
+      </c>
+      <c r="C503">
+        <v>25</v>
+      </c>
+      <c r="D503" t="s">
+        <v>30</v>
+      </c>
+      <c r="E503">
+        <v>100</v>
+      </c>
+      <c r="F503">
+        <v>71.5</v>
+      </c>
+      <c r="G503">
+        <v>76.2</v>
+      </c>
+      <c r="H503">
+        <v>100</v>
+      </c>
+      <c r="I503">
+        <v>100</v>
+      </c>
+      <c r="J503">
+        <v>75.099999999999994</v>
+      </c>
+      <c r="K503">
+        <v>78</v>
+      </c>
+      <c r="L503">
+        <v>83.3</v>
+      </c>
+      <c r="M503">
+        <v>19</v>
+      </c>
+      <c r="N503">
+        <v>84.2</v>
+      </c>
+      <c r="O503">
+        <v>7</v>
+      </c>
+      <c r="P503">
+        <v>88.3</v>
+      </c>
+      <c r="Q503">
+        <v>12</v>
+      </c>
+      <c r="R503">
+        <v>73.5</v>
+      </c>
+      <c r="S503">
+        <v>11</v>
+      </c>
+      <c r="T503">
+        <v>48.1</v>
+      </c>
+      <c r="U503">
+        <v>10</v>
+      </c>
+      <c r="V503">
+        <v>52.6</v>
+      </c>
+      <c r="W503">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="504" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A504" t="s">
+        <v>54</v>
+      </c>
+      <c r="B504" t="s">
+        <v>33</v>
+      </c>
+      <c r="C504">
+        <v>5</v>
+      </c>
+      <c r="D504" t="s">
+        <v>26</v>
+      </c>
+      <c r="E504">
+        <v>100</v>
+      </c>
+      <c r="F504">
+        <v>71.5</v>
+      </c>
+      <c r="G504">
+        <v>98.4</v>
+      </c>
+      <c r="H504">
+        <v>100</v>
+      </c>
+      <c r="I504">
+        <v>100</v>
+      </c>
+      <c r="J504">
+        <v>75.7</v>
+      </c>
+      <c r="K504">
+        <v>50</v>
+      </c>
+      <c r="L504">
+        <v>76.599999999999994</v>
+      </c>
+      <c r="M504">
+        <v>28</v>
+      </c>
+      <c r="N504">
+        <v>78.3</v>
+      </c>
+      <c r="O504">
+        <v>11</v>
+      </c>
+      <c r="P504">
+        <v>83.3</v>
+      </c>
+      <c r="Q504">
+        <v>12</v>
+      </c>
+      <c r="R504">
+        <v>89.7</v>
+      </c>
+      <c r="S504">
+        <v>5</v>
+      </c>
+      <c r="T504">
+        <v>37.5</v>
+      </c>
+      <c r="U504">
+        <v>14</v>
+      </c>
+      <c r="V504">
+        <v>40</v>
+      </c>
+      <c r="W504">
+        <v>13</v>
+      </c>
+      <c r="X504">
+        <v>40.299999999999997</v>
+      </c>
+      <c r="Y504">
+        <v>9</v>
+      </c>
+      <c r="Z504">
+        <v>40.799999999999997</v>
+      </c>
+      <c r="AA504">
+        <v>10</v>
+      </c>
+      <c r="AB504">
+        <v>41.8</v>
+      </c>
+      <c r="AC504">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="505" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A505" t="s">
+        <v>54</v>
+      </c>
+      <c r="B505" t="s">
+        <v>33</v>
+      </c>
+      <c r="C505">
+        <v>5</v>
+      </c>
+      <c r="D505" t="s">
+        <v>29</v>
+      </c>
+      <c r="E505">
+        <v>100</v>
+      </c>
+      <c r="F505">
+        <v>58.7</v>
+      </c>
+      <c r="G505">
+        <v>28.8</v>
+      </c>
+      <c r="H505">
+        <v>100</v>
+      </c>
+      <c r="I505">
+        <v>100</v>
+      </c>
+      <c r="J505">
+        <v>77.400000000000006</v>
+      </c>
+      <c r="K505">
+        <v>52</v>
+      </c>
+      <c r="L505">
+        <v>76.099999999999994</v>
+      </c>
+      <c r="M505">
+        <v>20</v>
+      </c>
+      <c r="N505">
+        <v>82.5</v>
+      </c>
+      <c r="O505">
+        <v>5</v>
+      </c>
+      <c r="P505">
+        <v>78.400000000000006</v>
+      </c>
+      <c r="Q505">
+        <v>5</v>
+      </c>
+      <c r="T505">
+        <v>34.9</v>
+      </c>
+      <c r="U505">
+        <v>44</v>
+      </c>
+      <c r="V505">
+        <v>41.7</v>
+      </c>
+      <c r="W505">
+        <v>13</v>
+      </c>
+      <c r="X505">
+        <v>39.5</v>
+      </c>
+      <c r="Y505">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="506" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A506" t="s">
+        <v>54</v>
+      </c>
+      <c r="B506" t="s">
+        <v>33</v>
+      </c>
+      <c r="C506">
+        <v>5</v>
+      </c>
+      <c r="D506" t="s">
+        <v>30</v>
+      </c>
+      <c r="E506">
+        <v>81.5</v>
+      </c>
+      <c r="F506">
+        <v>71.5</v>
+      </c>
+      <c r="G506">
+        <v>53.7</v>
+      </c>
+      <c r="H506">
+        <v>100</v>
+      </c>
+      <c r="I506">
+        <v>99.2</v>
+      </c>
+      <c r="J506">
+        <v>76</v>
+      </c>
+      <c r="K506">
+        <v>51</v>
+      </c>
+      <c r="L506">
+        <v>85.1</v>
+      </c>
+      <c r="M506">
+        <v>6</v>
+      </c>
+      <c r="N506">
+        <v>83.7</v>
+      </c>
+      <c r="O506">
+        <v>5</v>
+      </c>
+      <c r="P506">
+        <v>64.8</v>
+      </c>
+      <c r="Q506">
+        <v>13</v>
+      </c>
+      <c r="R506">
+        <v>61.5</v>
+      </c>
+      <c r="S506">
+        <v>5</v>
+      </c>
+      <c r="T506">
+        <v>43.2</v>
+      </c>
+      <c r="U506">
+        <v>5</v>
+      </c>
+      <c r="V506">
+        <v>38.9</v>
+      </c>
+      <c r="W506">
+        <v>7</v>
+      </c>
+      <c r="X506">
+        <v>29.7</v>
+      </c>
+      <c r="Y506">
+        <v>8</v>
+      </c>
+      <c r="Z506">
+        <v>29.7</v>
+      </c>
+      <c r="AA506">
+        <v>5</v>
+      </c>
+      <c r="AB506">
+        <v>23</v>
+      </c>
+      <c r="AC506">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="507" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A507" t="s">
+        <v>54</v>
+      </c>
+      <c r="B507" t="s">
+        <v>33</v>
+      </c>
+      <c r="C507">
+        <v>15</v>
+      </c>
+      <c r="D507" t="s">
+        <v>26</v>
+      </c>
+      <c r="E507">
+        <v>100</v>
+      </c>
+      <c r="F507">
+        <v>66.900000000000006</v>
+      </c>
+      <c r="G507">
+        <v>99.1</v>
+      </c>
+      <c r="H507">
+        <v>100</v>
+      </c>
+      <c r="I507">
+        <v>100</v>
+      </c>
+      <c r="J507">
+        <v>78</v>
+      </c>
+      <c r="K507">
+        <v>24</v>
+      </c>
+      <c r="L507">
+        <v>79.8</v>
+      </c>
+      <c r="M507">
+        <v>23</v>
+      </c>
+      <c r="N507">
+        <v>96.3</v>
+      </c>
+      <c r="O507">
+        <v>10</v>
+      </c>
+      <c r="P507">
+        <v>94.5</v>
+      </c>
+      <c r="Q507">
+        <v>7</v>
+      </c>
+      <c r="R507">
+        <v>86.9</v>
+      </c>
+      <c r="S507">
+        <v>8</v>
+      </c>
+      <c r="T507">
+        <v>34.6</v>
+      </c>
+      <c r="U507">
+        <v>27</v>
+      </c>
+      <c r="V507">
+        <v>36.200000000000003</v>
+      </c>
+      <c r="W507">
+        <v>12</v>
+      </c>
+      <c r="X507">
+        <v>36.5</v>
+      </c>
+      <c r="Y507">
+        <v>8</v>
+      </c>
+      <c r="Z507">
+        <v>38.799999999999997</v>
+      </c>
+      <c r="AA507">
+        <v>6</v>
+      </c>
+      <c r="AB507">
+        <v>34.200000000000003</v>
+      </c>
+      <c r="AC507">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="508" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A508" t="s">
+        <v>54</v>
+      </c>
+      <c r="B508" t="s">
+        <v>33</v>
+      </c>
+      <c r="C508">
+        <v>15</v>
+      </c>
+      <c r="D508" t="s">
+        <v>29</v>
+      </c>
+      <c r="E508">
+        <v>100</v>
+      </c>
+      <c r="F508">
+        <v>59.7</v>
+      </c>
+      <c r="G508">
+        <v>16.899999999999999</v>
+      </c>
+      <c r="H508">
+        <v>100</v>
+      </c>
+      <c r="I508">
+        <v>100</v>
+      </c>
+      <c r="J508">
+        <v>81.7</v>
+      </c>
+      <c r="K508">
+        <v>39</v>
+      </c>
+      <c r="L508">
+        <v>87.2</v>
+      </c>
+      <c r="M508">
+        <v>23</v>
+      </c>
+      <c r="N508">
+        <v>91.1</v>
+      </c>
+      <c r="O508">
+        <v>11</v>
+      </c>
+      <c r="T508">
+        <v>36.299999999999997</v>
+      </c>
+      <c r="U508">
+        <v>54</v>
+      </c>
+      <c r="V508">
+        <v>37</v>
+      </c>
+      <c r="W508">
+        <v>23</v>
+      </c>
+      <c r="X508">
+        <v>18.899999999999999</v>
+      </c>
+      <c r="Y508">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="509" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A509" t="s">
+        <v>54</v>
+      </c>
+      <c r="B509" t="s">
+        <v>33</v>
+      </c>
+      <c r="C509">
+        <v>15</v>
+      </c>
+      <c r="D509" t="s">
+        <v>30</v>
+      </c>
+      <c r="E509">
+        <v>99.5</v>
+      </c>
+      <c r="F509">
+        <v>71.5</v>
+      </c>
+      <c r="G509">
+        <v>73.099999999999994</v>
+      </c>
+      <c r="H509">
+        <v>100</v>
+      </c>
+      <c r="I509">
+        <v>99.7</v>
+      </c>
+      <c r="J509">
+        <v>75.8</v>
+      </c>
+      <c r="K509">
+        <v>43</v>
+      </c>
+      <c r="L509">
+        <v>92.2</v>
+      </c>
+      <c r="M509">
+        <v>8</v>
+      </c>
+      <c r="N509">
+        <v>96.1</v>
+      </c>
+      <c r="O509">
+        <v>6</v>
+      </c>
+      <c r="P509">
+        <v>97.6</v>
+      </c>
+      <c r="Q509">
+        <v>5</v>
+      </c>
+      <c r="R509">
+        <v>78.900000000000006</v>
+      </c>
+      <c r="S509">
+        <v>10</v>
+      </c>
+      <c r="T509">
+        <v>36.200000000000003</v>
+      </c>
+      <c r="U509">
+        <v>16</v>
+      </c>
+      <c r="V509">
+        <v>38.5</v>
+      </c>
+      <c r="W509">
+        <v>5</v>
+      </c>
+      <c r="X509">
+        <v>37.5</v>
+      </c>
+      <c r="Y509">
+        <v>5</v>
+      </c>
+      <c r="Z509">
+        <v>41.7</v>
+      </c>
+      <c r="AA509">
+        <v>5</v>
+      </c>
+      <c r="AB509">
+        <v>36.6</v>
+      </c>
+      <c r="AC509">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="510" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A510" t="s">
+        <v>54</v>
+      </c>
+      <c r="B510" t="s">
+        <v>33</v>
+      </c>
+      <c r="C510">
+        <v>25</v>
+      </c>
+      <c r="D510" t="s">
+        <v>26</v>
+      </c>
+      <c r="E510">
+        <v>100</v>
+      </c>
+      <c r="F510">
+        <v>67.599999999999994</v>
+      </c>
+      <c r="G510">
+        <v>99.4</v>
+      </c>
+      <c r="H510">
+        <v>100</v>
+      </c>
+      <c r="I510">
+        <v>100</v>
+      </c>
+      <c r="J510">
+        <v>76.2</v>
+      </c>
+      <c r="K510">
+        <v>63</v>
+      </c>
+      <c r="L510">
+        <v>79.2</v>
+      </c>
+      <c r="M510">
+        <v>26</v>
+      </c>
+      <c r="N510">
+        <v>87.3</v>
+      </c>
+      <c r="O510">
+        <v>10</v>
+      </c>
+      <c r="P510">
+        <v>78.599999999999994</v>
+      </c>
+      <c r="Q510">
+        <v>23</v>
+      </c>
+      <c r="R510">
+        <v>85.1</v>
+      </c>
+      <c r="S510">
+        <v>8</v>
+      </c>
+      <c r="T510">
+        <v>36.299999999999997</v>
+      </c>
+      <c r="U510">
+        <v>17</v>
+      </c>
+      <c r="V510">
+        <v>43.1</v>
+      </c>
+      <c r="W510">
+        <v>9</v>
+      </c>
+      <c r="X510">
+        <v>47.8</v>
+      </c>
+      <c r="Y510">
+        <v>6</v>
+      </c>
+      <c r="Z510">
+        <v>44.7</v>
+      </c>
+      <c r="AA510">
+        <v>5</v>
+      </c>
+      <c r="AB510">
+        <v>45.2</v>
+      </c>
+      <c r="AC510">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="511" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A511" t="s">
+        <v>54</v>
+      </c>
+      <c r="B511" t="s">
+        <v>33</v>
+      </c>
+      <c r="C511">
+        <v>25</v>
+      </c>
+      <c r="D511" t="s">
+        <v>29</v>
+      </c>
+      <c r="E511">
+        <v>100</v>
+      </c>
+      <c r="F511">
+        <v>59.9</v>
+      </c>
+      <c r="G511">
+        <v>14.1</v>
+      </c>
+      <c r="H511">
+        <v>100</v>
+      </c>
+      <c r="I511">
+        <v>100</v>
+      </c>
+      <c r="J511">
+        <v>83.4</v>
+      </c>
+      <c r="K511">
+        <v>38</v>
+      </c>
+      <c r="L511">
+        <v>88.5</v>
+      </c>
+      <c r="M511">
+        <v>18</v>
+      </c>
+      <c r="N511">
+        <v>91.9</v>
+      </c>
+      <c r="O511">
+        <v>8</v>
+      </c>
+      <c r="T511">
+        <v>36.6</v>
+      </c>
+      <c r="U511">
+        <v>44</v>
+      </c>
+      <c r="V511">
+        <v>40</v>
+      </c>
+      <c r="W511">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="512" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A512" t="s">
+        <v>54</v>
+      </c>
+      <c r="B512" t="s">
+        <v>33</v>
+      </c>
+      <c r="C512">
+        <v>25</v>
+      </c>
+      <c r="D512" t="s">
+        <v>30</v>
+      </c>
+      <c r="E512">
+        <v>100</v>
+      </c>
+      <c r="F512">
+        <v>71.5</v>
+      </c>
+      <c r="G512">
+        <v>66.2</v>
+      </c>
+      <c r="H512">
+        <v>100</v>
+      </c>
+      <c r="I512">
+        <v>100</v>
+      </c>
+      <c r="J512">
+        <v>79.599999999999994</v>
+      </c>
+      <c r="K512">
+        <v>29</v>
+      </c>
+      <c r="L512">
+        <v>94.1</v>
+      </c>
+      <c r="M512">
+        <v>9</v>
+      </c>
+      <c r="N512">
+        <v>95.8</v>
+      </c>
+      <c r="O512">
+        <v>6</v>
+      </c>
+      <c r="P512">
+        <v>92.3</v>
+      </c>
+      <c r="Q512">
+        <v>7</v>
+      </c>
+      <c r="R512">
+        <v>85.7</v>
+      </c>
+      <c r="S512">
+        <v>7</v>
+      </c>
+      <c r="T512">
+        <v>40</v>
+      </c>
+      <c r="U512">
+        <v>16</v>
+      </c>
+      <c r="V512">
+        <v>45.2</v>
+      </c>
+      <c r="W512">
+        <v>5</v>
+      </c>
+      <c r="X512">
+        <v>45.5</v>
+      </c>
+      <c r="Y512">
+        <v>7</v>
+      </c>
+      <c r="Z512">
+        <v>45.9</v>
+      </c>
+      <c r="AA512">
+        <v>8</v>
+      </c>
+      <c r="AB512">
+        <v>44.4</v>
+      </c>
+      <c r="AC512">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="513" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A513" t="s">
+        <v>54</v>
+      </c>
+      <c r="B513" t="s">
+        <v>34</v>
+      </c>
+      <c r="C513">
+        <v>5</v>
+      </c>
+      <c r="D513" t="s">
+        <v>26</v>
+      </c>
+      <c r="E513">
+        <v>99.1</v>
+      </c>
+      <c r="F513">
+        <v>71.099999999999994</v>
+      </c>
+      <c r="G513">
+        <v>95.6</v>
+      </c>
+      <c r="H513">
+        <v>98.8</v>
+      </c>
+      <c r="I513">
+        <v>99.4</v>
+      </c>
+      <c r="J513">
+        <v>89.4</v>
+      </c>
+      <c r="K513">
+        <v>18</v>
+      </c>
+      <c r="L513">
+        <v>93.5</v>
+      </c>
+      <c r="M513">
+        <v>8</v>
+      </c>
+      <c r="N513">
+        <v>98.4</v>
+      </c>
+      <c r="O513">
+        <v>8</v>
+      </c>
+      <c r="P513">
+        <v>100</v>
+      </c>
+      <c r="Q513">
+        <v>5</v>
+      </c>
+      <c r="R513">
+        <v>92.9</v>
+      </c>
+      <c r="S513">
+        <v>5</v>
+      </c>
+      <c r="T513">
+        <v>40.700000000000003</v>
+      </c>
+      <c r="U513">
+        <v>35</v>
+      </c>
+      <c r="V513">
+        <v>37</v>
+      </c>
+      <c r="W513">
+        <v>13</v>
+      </c>
+      <c r="X513">
+        <v>44</v>
+      </c>
+      <c r="Y513">
+        <v>6</v>
+      </c>
+      <c r="Z513">
+        <v>36.9</v>
+      </c>
+      <c r="AA513">
+        <v>8</v>
+      </c>
+      <c r="AB513">
+        <v>38.299999999999997</v>
+      </c>
+      <c r="AC513">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="514" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A514" t="s">
+        <v>54</v>
+      </c>
+      <c r="B514" t="s">
+        <v>34</v>
+      </c>
+      <c r="C514">
+        <v>5</v>
+      </c>
+      <c r="D514" t="s">
+        <v>29</v>
+      </c>
+      <c r="E514">
+        <v>100</v>
+      </c>
+      <c r="F514">
+        <v>62.2</v>
+      </c>
+      <c r="G514">
+        <v>31.3</v>
+      </c>
+      <c r="H514">
+        <v>100</v>
+      </c>
+      <c r="I514">
+        <v>100</v>
+      </c>
+      <c r="J514">
+        <v>81</v>
+      </c>
+      <c r="K514">
+        <v>51</v>
+      </c>
+      <c r="L514">
+        <v>86.9</v>
+      </c>
+      <c r="M514">
+        <v>20</v>
+      </c>
+      <c r="N514">
+        <v>90.2</v>
+      </c>
+      <c r="O514">
+        <v>12</v>
+      </c>
+      <c r="P514">
+        <v>100</v>
+      </c>
+      <c r="Q514">
+        <v>5</v>
+      </c>
+      <c r="T514">
+        <v>38.4</v>
+      </c>
+      <c r="U514">
+        <v>49</v>
+      </c>
+      <c r="V514">
+        <v>37.799999999999997</v>
+      </c>
+      <c r="W514">
+        <v>15</v>
+      </c>
+      <c r="X514">
+        <v>38.1</v>
+      </c>
+      <c r="Y514">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="515" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A515" t="s">
+        <v>54</v>
+      </c>
+      <c r="B515" t="s">
+        <v>34</v>
+      </c>
+      <c r="C515">
+        <v>5</v>
+      </c>
+      <c r="D515" t="s">
+        <v>30</v>
+      </c>
+      <c r="E515">
+        <v>70.7</v>
+      </c>
+      <c r="F515">
+        <v>71.5</v>
+      </c>
+      <c r="G515">
+        <v>9.6</v>
+      </c>
+      <c r="H515">
+        <v>100</v>
+      </c>
+      <c r="I515">
+        <v>96.2</v>
+      </c>
+      <c r="J515">
+        <v>80.7</v>
+      </c>
+      <c r="K515">
+        <v>37</v>
+      </c>
+      <c r="L515">
+        <v>86.3</v>
+      </c>
+      <c r="M515">
+        <v>19</v>
+      </c>
+      <c r="N515">
+        <v>98.4</v>
+      </c>
+      <c r="O515">
+        <v>8</v>
+      </c>
+      <c r="T515">
+        <v>38.299999999999997</v>
+      </c>
+      <c r="U515">
+        <v>14</v>
+      </c>
+      <c r="V515">
+        <v>35.1</v>
+      </c>
+      <c r="W515">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="516" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A516" t="s">
+        <v>54</v>
+      </c>
+      <c r="B516" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C516" s="3">
+        <v>15</v>
+      </c>
+      <c r="D516" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E516">
+        <v>100</v>
+      </c>
+      <c r="F516">
+        <v>71.5</v>
+      </c>
+      <c r="G516">
+        <v>98.5</v>
+      </c>
+      <c r="H516">
+        <v>100</v>
+      </c>
+      <c r="I516">
+        <v>100</v>
+      </c>
+      <c r="J516">
+        <v>80.8</v>
+      </c>
+      <c r="K516">
+        <v>15</v>
+      </c>
+      <c r="L516">
+        <v>77</v>
+      </c>
+      <c r="M516">
+        <v>50</v>
+      </c>
+      <c r="N516">
+        <v>80.8</v>
+      </c>
+      <c r="O516">
+        <v>30</v>
+      </c>
+      <c r="P516">
+        <v>90.6</v>
+      </c>
+      <c r="Q516">
+        <v>8</v>
+      </c>
+      <c r="R516">
+        <v>90.9</v>
+      </c>
+      <c r="S516">
+        <v>7</v>
+      </c>
+      <c r="T516">
+        <v>38.200000000000003</v>
+      </c>
+      <c r="U516">
+        <v>22</v>
+      </c>
+      <c r="V516">
+        <v>44.4</v>
+      </c>
+      <c r="W516">
+        <v>8</v>
+      </c>
+      <c r="X516">
+        <v>42</v>
+      </c>
+      <c r="Y516">
+        <v>6</v>
+      </c>
+      <c r="Z516">
+        <v>39.299999999999997</v>
+      </c>
+      <c r="AA516">
+        <v>15</v>
+      </c>
+      <c r="AB516">
+        <v>43.7</v>
+      </c>
+      <c r="AC516">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="517" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A517" t="s">
+        <v>54</v>
+      </c>
+      <c r="B517" t="s">
+        <v>34</v>
+      </c>
+      <c r="C517">
+        <v>15</v>
+      </c>
+      <c r="D517" t="s">
+        <v>29</v>
+      </c>
+      <c r="E517">
+        <v>100</v>
+      </c>
+      <c r="F517">
+        <v>63.9</v>
+      </c>
+      <c r="G517">
+        <v>25.2</v>
+      </c>
+      <c r="H517">
+        <v>100</v>
+      </c>
+      <c r="I517">
+        <v>100</v>
+      </c>
+      <c r="J517">
+        <v>73.7</v>
+      </c>
+      <c r="K517">
+        <v>64</v>
+      </c>
+      <c r="L517">
+        <v>85.8</v>
+      </c>
+      <c r="M517">
+        <v>23</v>
+      </c>
+      <c r="N517">
+        <v>92.4</v>
+      </c>
+      <c r="O517">
+        <v>12</v>
+      </c>
+      <c r="P517">
+        <v>86.1</v>
+      </c>
+      <c r="Q517">
+        <v>5</v>
+      </c>
+      <c r="T517">
+        <v>31.8</v>
+      </c>
+      <c r="U517">
+        <v>36</v>
+      </c>
+      <c r="V517">
+        <v>39.5</v>
+      </c>
+      <c r="W517">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="518" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A518" t="s">
+        <v>54</v>
+      </c>
+      <c r="B518" t="s">
+        <v>34</v>
+      </c>
+      <c r="C518">
+        <v>15</v>
+      </c>
+      <c r="D518" t="s">
+        <v>30</v>
+      </c>
+      <c r="E518">
+        <v>100</v>
+      </c>
+      <c r="F518">
+        <v>71.599999999999994</v>
+      </c>
+      <c r="G518">
+        <v>71.2</v>
+      </c>
+      <c r="H518">
+        <v>100</v>
+      </c>
+      <c r="I518">
+        <v>100</v>
+      </c>
+      <c r="J518">
+        <v>75.599999999999994</v>
+      </c>
+      <c r="K518">
+        <v>59</v>
+      </c>
+      <c r="L518">
+        <v>83.7</v>
+      </c>
+      <c r="M518">
+        <v>13</v>
+      </c>
+      <c r="N518">
+        <v>88.9</v>
+      </c>
+      <c r="O518">
+        <v>5</v>
+      </c>
+      <c r="P518">
+        <v>91</v>
+      </c>
+      <c r="Q518">
+        <v>10</v>
+      </c>
+      <c r="R518">
+        <v>95</v>
+      </c>
+      <c r="S518">
+        <v>5</v>
+      </c>
+      <c r="T518">
+        <v>39.1</v>
+      </c>
+      <c r="U518">
+        <v>8</v>
+      </c>
+      <c r="V518">
+        <v>43.3</v>
+      </c>
+      <c r="W518">
+        <v>8</v>
+      </c>
+      <c r="X518">
+        <v>42.9</v>
+      </c>
+      <c r="Y518">
+        <v>5</v>
+      </c>
+      <c r="Z518">
+        <v>33.299999999999997</v>
+      </c>
+      <c r="AA518">
+        <v>7</v>
+      </c>
+      <c r="AB518">
+        <v>35</v>
+      </c>
+      <c r="AC518">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="519" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A519" t="s">
+        <v>54</v>
+      </c>
+      <c r="B519" t="s">
+        <v>34</v>
+      </c>
+      <c r="C519">
+        <v>25</v>
+      </c>
+      <c r="D519" t="s">
+        <v>26</v>
+      </c>
+      <c r="E519">
+        <v>100</v>
+      </c>
+      <c r="F519">
+        <v>65.7</v>
+      </c>
+      <c r="G519">
+        <v>99.6</v>
+      </c>
+      <c r="H519">
+        <v>100</v>
+      </c>
+      <c r="I519">
+        <v>100</v>
+      </c>
+      <c r="J519">
+        <v>75.400000000000006</v>
+      </c>
+      <c r="K519">
+        <v>62</v>
+      </c>
+      <c r="L519">
+        <v>77</v>
+      </c>
+      <c r="M519">
+        <v>47</v>
+      </c>
+      <c r="N519">
+        <v>76.900000000000006</v>
+      </c>
+      <c r="O519">
+        <v>37</v>
+      </c>
+      <c r="P519">
+        <v>78.900000000000006</v>
+      </c>
+      <c r="Q519">
+        <v>34</v>
+      </c>
+      <c r="R519">
+        <v>90</v>
+      </c>
+      <c r="S519">
+        <v>5</v>
+      </c>
+      <c r="T519">
+        <v>34.4</v>
+      </c>
+      <c r="U519">
+        <v>38</v>
+      </c>
+      <c r="V519">
+        <v>36.799999999999997</v>
+      </c>
+      <c r="W519">
+        <v>23</v>
+      </c>
+      <c r="X519">
+        <v>35.700000000000003</v>
+      </c>
+      <c r="Y519">
+        <v>32</v>
+      </c>
+      <c r="Z519">
+        <v>37.5</v>
+      </c>
+      <c r="AA519">
+        <v>6</v>
+      </c>
+      <c r="AB519">
+        <v>36</v>
+      </c>
+      <c r="AC519">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="520" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A520" t="s">
+        <v>54</v>
+      </c>
+      <c r="B520" t="s">
+        <v>34</v>
+      </c>
+      <c r="C520">
+        <v>25</v>
+      </c>
+      <c r="D520" t="s">
+        <v>29</v>
+      </c>
+      <c r="E520">
+        <v>100</v>
+      </c>
+      <c r="F520">
+        <v>62.9</v>
+      </c>
+      <c r="G520">
+        <v>25.6</v>
+      </c>
+      <c r="H520">
+        <v>100</v>
+      </c>
+      <c r="I520">
+        <v>100</v>
+      </c>
+      <c r="J520">
+        <v>72.7</v>
+      </c>
+      <c r="K520">
+        <v>67</v>
+      </c>
+      <c r="L520">
+        <v>87.6</v>
+      </c>
+      <c r="M520">
+        <v>23</v>
+      </c>
+      <c r="N520">
+        <v>90.9</v>
+      </c>
+      <c r="O520">
+        <v>13</v>
+      </c>
+      <c r="P520">
+        <v>94.7</v>
+      </c>
+      <c r="Q520">
+        <v>5</v>
+      </c>
+      <c r="T520">
+        <v>30.2</v>
+      </c>
+      <c r="U520">
+        <v>33</v>
+      </c>
+      <c r="V520">
+        <v>30.4</v>
+      </c>
+      <c r="W520">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="521" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A521" t="s">
+        <v>54</v>
+      </c>
+      <c r="B521" t="s">
+        <v>34</v>
+      </c>
+      <c r="C521">
+        <v>25</v>
+      </c>
+      <c r="D521" t="s">
+        <v>30</v>
+      </c>
+      <c r="E521">
+        <v>100</v>
+      </c>
+      <c r="F521">
+        <v>71.5</v>
+      </c>
+      <c r="G521">
+        <v>73.099999999999994</v>
+      </c>
+      <c r="H521">
+        <v>100</v>
+      </c>
+      <c r="I521">
+        <v>100</v>
+      </c>
+      <c r="J521">
+        <v>75.7</v>
+      </c>
+      <c r="K521">
+        <v>52</v>
+      </c>
+      <c r="L521">
+        <v>82.3</v>
+      </c>
+      <c r="M521">
+        <v>23</v>
+      </c>
+      <c r="N521">
+        <v>89.3</v>
+      </c>
+      <c r="O521">
+        <v>11</v>
+      </c>
+      <c r="P521">
+        <v>93.6</v>
+      </c>
+      <c r="Q521">
+        <v>6</v>
+      </c>
+      <c r="R521">
+        <v>87.8</v>
+      </c>
+      <c r="S521">
+        <v>6</v>
+      </c>
+      <c r="T521">
+        <v>38.200000000000003</v>
+      </c>
+      <c r="U521">
+        <v>23</v>
+      </c>
+      <c r="V521">
+        <v>40.5</v>
+      </c>
+      <c r="W521">
+        <v>5</v>
+      </c>
+      <c r="X521">
+        <v>40</v>
+      </c>
+      <c r="Y521">
+        <v>5</v>
+      </c>
+      <c r="Z521">
+        <v>40.5</v>
+      </c>
+      <c r="AA521">
+        <v>5</v>
+      </c>
+      <c r="AB521">
+        <v>35.1</v>
+      </c>
+      <c r="AC521">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
7majors high plus 1 atr
undersample test and train
</commit_message>
<xml_diff>
--- a/wm/Results.xlsx
+++ b/wm/Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pioo\notebooks\wm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F68048CC-2C2F-4CCC-966A-DF2405998F1D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B0C5AA1-884A-45C6-883F-4BFBAA2D060D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView minimized="1" xWindow="690" yWindow="2640" windowWidth="26010" windowHeight="11385" tabRatio="435" xr2:uid="{B6B0453F-83A4-43EC-A328-DC10FEB5BD2E}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$AC$1103</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$AC$1109</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3353" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3407" uniqueCount="80">
   <si>
     <t>Te_cal</t>
   </si>
@@ -250,6 +250,33 @@
   </si>
   <si>
     <t>test20_16c</t>
+  </si>
+  <si>
+    <t>test21_10c</t>
+  </si>
+  <si>
+    <t>test21_14c</t>
+  </si>
+  <si>
+    <t>test21_16c</t>
+  </si>
+  <si>
+    <t>test22_10c</t>
+  </si>
+  <si>
+    <t>test22_14c</t>
+  </si>
+  <si>
+    <t>test22_16c</t>
+  </si>
+  <si>
+    <t>test23_10c</t>
+  </si>
+  <si>
+    <t>test23_14c</t>
+  </si>
+  <si>
+    <t>test23_16c</t>
   </si>
 </sst>
 </file>
@@ -659,13 +686,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBA71D6A-A9B1-42AC-9396-7E4A540CDDDA}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:AC1109"/>
+  <dimension ref="A1:AC1127"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E1070" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E1102" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E1110" sqref="E1110"/>
+      <selection pane="bottomRight" activeCell="M1134" sqref="M1134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -85931,9 +85958,1402 @@
         <v>10</v>
       </c>
     </row>
+    <row r="1110" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1110" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1110" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1110" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1110">
+        <v>100</v>
+      </c>
+      <c r="F1110">
+        <v>65.599999999999994</v>
+      </c>
+      <c r="G1110">
+        <v>85.4</v>
+      </c>
+      <c r="H1110">
+        <v>0</v>
+      </c>
+      <c r="I1110">
+        <v>0</v>
+      </c>
+      <c r="J1110">
+        <v>67.400000000000006</v>
+      </c>
+      <c r="K1110">
+        <v>43</v>
+      </c>
+      <c r="L1110">
+        <v>78.900000000000006</v>
+      </c>
+      <c r="M1110">
+        <v>12</v>
+      </c>
+      <c r="N1110">
+        <v>84.8</v>
+      </c>
+      <c r="O1110">
+        <v>11</v>
+      </c>
+      <c r="P1110">
+        <v>83.9</v>
+      </c>
+      <c r="Q1110">
+        <v>10</v>
+      </c>
+      <c r="R1110">
+        <v>87.9</v>
+      </c>
+      <c r="S1110">
+        <v>11</v>
+      </c>
+      <c r="T1110">
+        <v>75.599999999999994</v>
+      </c>
+      <c r="U1110">
+        <v>27</v>
+      </c>
+      <c r="V1110">
+        <v>80.5</v>
+      </c>
+      <c r="W1110">
+        <v>13</v>
+      </c>
+      <c r="X1110">
+        <v>87.1</v>
+      </c>
+      <c r="Y1110">
+        <v>10</v>
+      </c>
+      <c r="Z1110">
+        <v>84.4</v>
+      </c>
+      <c r="AA1110">
+        <v>10</v>
+      </c>
+      <c r="AB1110">
+        <v>84.4</v>
+      </c>
+      <c r="AC1110">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1111" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1111" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1111" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1111" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1111">
+        <v>100</v>
+      </c>
+      <c r="F1111">
+        <v>61.8</v>
+      </c>
+      <c r="G1111">
+        <v>25.5</v>
+      </c>
+      <c r="H1111">
+        <v>100</v>
+      </c>
+      <c r="I1111">
+        <v>100</v>
+      </c>
+      <c r="J1111">
+        <v>74</v>
+      </c>
+      <c r="K1111">
+        <v>16</v>
+      </c>
+      <c r="L1111">
+        <v>72</v>
+      </c>
+      <c r="M1111">
+        <v>16</v>
+      </c>
+      <c r="N1111">
+        <v>81.8</v>
+      </c>
+      <c r="O1111">
+        <v>11</v>
+      </c>
+      <c r="S1111"/>
+      <c r="T1111">
+        <v>61.3</v>
+      </c>
+      <c r="U1111">
+        <v>45</v>
+      </c>
+      <c r="V1111">
+        <v>76.3</v>
+      </c>
+      <c r="W1111">
+        <v>19</v>
+      </c>
+      <c r="X1111">
+        <v>80.599999999999994</v>
+      </c>
+      <c r="Y1111">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1112" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1112" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1112" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1112" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1112">
+        <v>100</v>
+      </c>
+      <c r="F1112">
+        <v>67.8</v>
+      </c>
+      <c r="G1112">
+        <v>79.8</v>
+      </c>
+      <c r="H1112">
+        <v>0</v>
+      </c>
+      <c r="I1112">
+        <v>0</v>
+      </c>
+      <c r="J1112">
+        <v>66</v>
+      </c>
+      <c r="K1112">
+        <v>54</v>
+      </c>
+      <c r="L1112">
+        <v>71.900000000000006</v>
+      </c>
+      <c r="M1112">
+        <v>33</v>
+      </c>
+      <c r="N1112">
+        <v>77</v>
+      </c>
+      <c r="O1112">
+        <v>23</v>
+      </c>
+      <c r="P1112">
+        <v>85.7</v>
+      </c>
+      <c r="Q1112">
+        <v>10</v>
+      </c>
+      <c r="R1112">
+        <v>88.5</v>
+      </c>
+      <c r="S1112">
+        <v>10</v>
+      </c>
+      <c r="T1112">
+        <v>76.7</v>
+      </c>
+      <c r="U1112">
+        <v>22</v>
+      </c>
+      <c r="V1112">
+        <v>87.1</v>
+      </c>
+      <c r="W1112">
+        <v>12</v>
+      </c>
+      <c r="X1112">
+        <v>89.3</v>
+      </c>
+      <c r="Y1112">
+        <v>10</v>
+      </c>
+      <c r="Z1112">
+        <v>82.1</v>
+      </c>
+      <c r="AA1112">
+        <v>10</v>
+      </c>
+      <c r="AB1112">
+        <v>83.9</v>
+      </c>
+      <c r="AC1112">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1113" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1113" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1113" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1113" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1113">
+        <v>100</v>
+      </c>
+      <c r="F1113">
+        <v>65.900000000000006</v>
+      </c>
+      <c r="G1113">
+        <v>27</v>
+      </c>
+      <c r="H1113">
+        <v>100</v>
+      </c>
+      <c r="I1113">
+        <v>100</v>
+      </c>
+      <c r="J1113">
+        <v>66.3</v>
+      </c>
+      <c r="K1113">
+        <v>37</v>
+      </c>
+      <c r="L1113">
+        <v>71.8</v>
+      </c>
+      <c r="M1113">
+        <v>32</v>
+      </c>
+      <c r="N1113">
+        <v>85.7</v>
+      </c>
+      <c r="O1113">
+        <v>13</v>
+      </c>
+      <c r="S1113"/>
+      <c r="T1113">
+        <v>69.3</v>
+      </c>
+      <c r="U1113">
+        <v>38</v>
+      </c>
+      <c r="V1113">
+        <v>83.8</v>
+      </c>
+      <c r="W1113">
+        <v>14</v>
+      </c>
+      <c r="X1113">
+        <v>66.7</v>
+      </c>
+      <c r="Y1113">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1114" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1114" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1114" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1114" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1114">
+        <v>99.2</v>
+      </c>
+      <c r="F1114">
+        <v>66.7</v>
+      </c>
+      <c r="G1114">
+        <v>80.2</v>
+      </c>
+      <c r="H1114">
+        <v>0</v>
+      </c>
+      <c r="I1114">
+        <v>0</v>
+      </c>
+      <c r="J1114">
+        <v>72.400000000000006</v>
+      </c>
+      <c r="K1114">
+        <v>38</v>
+      </c>
+      <c r="L1114">
+        <v>78.3</v>
+      </c>
+      <c r="M1114">
+        <v>27</v>
+      </c>
+      <c r="N1114">
+        <v>90.9</v>
+      </c>
+      <c r="O1114">
+        <v>11</v>
+      </c>
+      <c r="P1114">
+        <v>88.6</v>
+      </c>
+      <c r="Q1114">
+        <v>12</v>
+      </c>
+      <c r="R1114">
+        <v>90</v>
+      </c>
+      <c r="S1114">
+        <v>10</v>
+      </c>
+      <c r="T1114">
+        <v>75</v>
+      </c>
+      <c r="U1114">
+        <v>13</v>
+      </c>
+      <c r="V1114">
+        <v>86.7</v>
+      </c>
+      <c r="W1114">
+        <v>10</v>
+      </c>
+      <c r="X1114">
+        <v>85.7</v>
+      </c>
+      <c r="Y1114">
+        <v>16</v>
+      </c>
+      <c r="Z1114">
+        <v>87.1</v>
+      </c>
+      <c r="AA1114">
+        <v>10</v>
+      </c>
+      <c r="AB1114">
+        <v>86.8</v>
+      </c>
+      <c r="AC1114">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1115" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1115" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1115" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1115" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1115">
+        <v>100</v>
+      </c>
+      <c r="F1115">
+        <v>64.7</v>
+      </c>
+      <c r="G1115">
+        <v>60.7</v>
+      </c>
+      <c r="H1115">
+        <v>100</v>
+      </c>
+      <c r="I1115">
+        <v>100</v>
+      </c>
+      <c r="J1115">
+        <v>68</v>
+      </c>
+      <c r="K1115">
+        <v>40</v>
+      </c>
+      <c r="L1115">
+        <v>86.7</v>
+      </c>
+      <c r="M1115">
+        <v>20</v>
+      </c>
+      <c r="N1115">
+        <v>82.8</v>
+      </c>
+      <c r="O1115">
+        <v>10</v>
+      </c>
+      <c r="P1115">
+        <v>67.3</v>
+      </c>
+      <c r="Q1115">
+        <v>17</v>
+      </c>
+      <c r="S1115"/>
+      <c r="T1115">
+        <v>65.5</v>
+      </c>
+      <c r="U1115">
+        <v>36</v>
+      </c>
+      <c r="V1115">
+        <v>76.7</v>
+      </c>
+      <c r="W1115">
+        <v>10</v>
+      </c>
+      <c r="X1115">
+        <v>79.5</v>
+      </c>
+      <c r="Y1115">
+        <v>13</v>
+      </c>
+      <c r="Z1115">
+        <v>78.8</v>
+      </c>
+      <c r="AA1115">
+        <v>11</v>
+      </c>
+      <c r="AB1115">
+        <v>66.7</v>
+      </c>
+      <c r="AC1115">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1116" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1116" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1116" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1116" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1116">
+        <v>100</v>
+      </c>
+      <c r="F1116">
+        <v>77.8</v>
+      </c>
+      <c r="G1116">
+        <v>98.6</v>
+      </c>
+      <c r="H1116">
+        <v>0</v>
+      </c>
+      <c r="I1116">
+        <v>0</v>
+      </c>
+      <c r="J1116">
+        <v>88.2</v>
+      </c>
+      <c r="K1116">
+        <v>24</v>
+      </c>
+      <c r="L1116">
+        <v>92.9</v>
+      </c>
+      <c r="M1116">
+        <v>19</v>
+      </c>
+      <c r="N1116">
+        <v>91.7</v>
+      </c>
+      <c r="O1116">
+        <v>17</v>
+      </c>
+      <c r="P1116">
+        <v>92.9</v>
+      </c>
+      <c r="Q1116">
+        <v>19</v>
+      </c>
+      <c r="R1116">
+        <v>94.7</v>
+      </c>
+      <c r="S1116">
+        <v>26</v>
+      </c>
+      <c r="T1116">
+        <v>91.7</v>
+      </c>
+      <c r="U1116">
+        <v>17</v>
+      </c>
+      <c r="V1116">
+        <v>100</v>
+      </c>
+      <c r="W1116">
+        <v>10</v>
+      </c>
+      <c r="X1116">
+        <v>100</v>
+      </c>
+      <c r="Y1116">
+        <v>14</v>
+      </c>
+      <c r="Z1116">
+        <v>100</v>
+      </c>
+      <c r="AA1116">
+        <v>10</v>
+      </c>
+      <c r="AB1116">
+        <v>100</v>
+      </c>
+      <c r="AC1116">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1117" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1117" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1117" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1117" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1117">
+        <v>100</v>
+      </c>
+      <c r="F1117">
+        <v>69.400000000000006</v>
+      </c>
+      <c r="G1117">
+        <v>4.2</v>
+      </c>
+      <c r="H1117">
+        <v>100</v>
+      </c>
+      <c r="I1117">
+        <v>100</v>
+      </c>
+      <c r="J1117">
+        <v>100</v>
+      </c>
+      <c r="K1117">
+        <v>10</v>
+      </c>
+      <c r="L1117">
+        <v>100</v>
+      </c>
+      <c r="M1117">
+        <v>11</v>
+      </c>
+      <c r="S1117"/>
+      <c r="T1117">
+        <v>72</v>
+      </c>
+      <c r="U1117">
+        <v>35</v>
+      </c>
+      <c r="V1117">
+        <v>87.5</v>
+      </c>
+      <c r="W1117">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1118" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1118" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1118" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1118" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1118">
+        <v>100</v>
+      </c>
+      <c r="F1118">
+        <v>83.3</v>
+      </c>
+      <c r="G1118">
+        <v>98.3</v>
+      </c>
+      <c r="H1118">
+        <v>0</v>
+      </c>
+      <c r="I1118">
+        <v>0</v>
+      </c>
+      <c r="J1118">
+        <v>100</v>
+      </c>
+      <c r="K1118">
+        <v>17</v>
+      </c>
+      <c r="L1118">
+        <v>100</v>
+      </c>
+      <c r="M1118">
+        <v>17</v>
+      </c>
+      <c r="N1118">
+        <v>100</v>
+      </c>
+      <c r="O1118">
+        <v>17</v>
+      </c>
+      <c r="P1118">
+        <v>100</v>
+      </c>
+      <c r="Q1118">
+        <v>17</v>
+      </c>
+      <c r="R1118">
+        <v>100</v>
+      </c>
+      <c r="S1118">
+        <v>17</v>
+      </c>
+      <c r="T1118">
+        <v>88.2</v>
+      </c>
+      <c r="U1118">
+        <v>28</v>
+      </c>
+      <c r="V1118">
+        <v>92.3</v>
+      </c>
+      <c r="W1118">
+        <v>22</v>
+      </c>
+      <c r="X1118">
+        <v>100</v>
+      </c>
+      <c r="Y1118">
+        <v>10</v>
+      </c>
+      <c r="Z1118">
+        <v>90.9</v>
+      </c>
+      <c r="AA1118">
+        <v>18</v>
+      </c>
+      <c r="AB1118">
+        <v>92.9</v>
+      </c>
+      <c r="AC1118">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="1119" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1119" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1119" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1119" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1119">
+        <v>100</v>
+      </c>
+      <c r="F1119">
+        <v>76.7</v>
+      </c>
+      <c r="G1119">
+        <v>33.299999999999997</v>
+      </c>
+      <c r="H1119">
+        <v>100</v>
+      </c>
+      <c r="I1119">
+        <v>100</v>
+      </c>
+      <c r="J1119">
+        <v>77.3</v>
+      </c>
+      <c r="K1119">
+        <v>37</v>
+      </c>
+      <c r="L1119">
+        <v>100</v>
+      </c>
+      <c r="M1119">
+        <v>10</v>
+      </c>
+      <c r="N1119">
+        <v>100</v>
+      </c>
+      <c r="O1119">
+        <v>13</v>
+      </c>
+      <c r="S1119"/>
+      <c r="T1119">
+        <v>87.5</v>
+      </c>
+      <c r="U1119">
+        <v>40</v>
+      </c>
+      <c r="V1119">
+        <v>91.7</v>
+      </c>
+      <c r="W1119">
+        <v>20</v>
+      </c>
+      <c r="X1119">
+        <v>87.5</v>
+      </c>
+      <c r="Y1119">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1120" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1120" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1120" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1120" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1120">
+        <v>98.4</v>
+      </c>
+      <c r="F1120">
+        <v>80.3</v>
+      </c>
+      <c r="G1120">
+        <v>97</v>
+      </c>
+      <c r="H1120">
+        <v>0</v>
+      </c>
+      <c r="I1120">
+        <v>0</v>
+      </c>
+      <c r="J1120">
+        <v>100</v>
+      </c>
+      <c r="K1120">
+        <v>24</v>
+      </c>
+      <c r="L1120">
+        <v>100</v>
+      </c>
+      <c r="M1120">
+        <v>23</v>
+      </c>
+      <c r="N1120">
+        <v>100</v>
+      </c>
+      <c r="O1120">
+        <v>20</v>
+      </c>
+      <c r="P1120">
+        <v>100</v>
+      </c>
+      <c r="Q1120">
+        <v>14</v>
+      </c>
+      <c r="R1120">
+        <v>100</v>
+      </c>
+      <c r="S1120">
+        <v>14</v>
+      </c>
+      <c r="T1120">
+        <v>85.7</v>
+      </c>
+      <c r="U1120">
+        <v>21</v>
+      </c>
+      <c r="V1120">
+        <v>87.5</v>
+      </c>
+      <c r="W1120">
+        <v>12</v>
+      </c>
+      <c r="X1120">
+        <v>87.5</v>
+      </c>
+      <c r="Y1120">
+        <v>12</v>
+      </c>
+      <c r="Z1120">
+        <v>90</v>
+      </c>
+      <c r="AA1120">
+        <v>15</v>
+      </c>
+      <c r="AB1120">
+        <v>100</v>
+      </c>
+      <c r="AC1120">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1121" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1121" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1121" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1121" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1121">
+        <v>100</v>
+      </c>
+      <c r="F1121">
+        <v>77.3</v>
+      </c>
+      <c r="G1121">
+        <v>69.7</v>
+      </c>
+      <c r="H1121">
+        <v>100</v>
+      </c>
+      <c r="I1121">
+        <v>100</v>
+      </c>
+      <c r="J1121">
+        <v>100</v>
+      </c>
+      <c r="K1121">
+        <v>12</v>
+      </c>
+      <c r="L1121">
+        <v>100</v>
+      </c>
+      <c r="M1121">
+        <v>24</v>
+      </c>
+      <c r="N1121">
+        <v>100</v>
+      </c>
+      <c r="O1121">
+        <v>11</v>
+      </c>
+      <c r="P1121">
+        <v>100</v>
+      </c>
+      <c r="Q1121">
+        <v>11</v>
+      </c>
+      <c r="R1121">
+        <v>71.400000000000006</v>
+      </c>
+      <c r="S1121">
+        <v>11</v>
+      </c>
+      <c r="T1121">
+        <v>71.400000000000006</v>
+      </c>
+      <c r="U1121">
+        <v>21</v>
+      </c>
+      <c r="V1121">
+        <v>80</v>
+      </c>
+      <c r="W1121">
+        <v>23</v>
+      </c>
+      <c r="X1121">
+        <v>88.9</v>
+      </c>
+      <c r="Y1121">
+        <v>14</v>
+      </c>
+      <c r="Z1121">
+        <v>88.9</v>
+      </c>
+      <c r="AA1121">
+        <v>14</v>
+      </c>
+      <c r="AB1121">
+        <v>85.7</v>
+      </c>
+      <c r="AC1121">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1122" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1122" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1122" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1122" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1122">
+        <v>100</v>
+      </c>
+      <c r="F1122">
+        <v>61.4</v>
+      </c>
+      <c r="G1122">
+        <v>82.2</v>
+      </c>
+      <c r="H1122">
+        <v>0</v>
+      </c>
+      <c r="I1122">
+        <v>0</v>
+      </c>
+      <c r="J1122">
+        <v>69.599999999999994</v>
+      </c>
+      <c r="K1122">
+        <v>19</v>
+      </c>
+      <c r="L1122">
+        <v>74.5</v>
+      </c>
+      <c r="M1122">
+        <v>10</v>
+      </c>
+      <c r="N1122">
+        <v>73.8</v>
+      </c>
+      <c r="O1122">
+        <v>16</v>
+      </c>
+      <c r="P1122">
+        <v>78.8</v>
+      </c>
+      <c r="Q1122">
+        <v>11</v>
+      </c>
+      <c r="R1122">
+        <v>73.099999999999994</v>
+      </c>
+      <c r="S1122">
+        <v>11</v>
+      </c>
+      <c r="T1122">
+        <v>69.2</v>
+      </c>
+      <c r="U1122">
+        <v>16</v>
+      </c>
+      <c r="V1122">
+        <v>74.5</v>
+      </c>
+      <c r="W1122">
+        <v>11</v>
+      </c>
+      <c r="X1122">
+        <v>78</v>
+      </c>
+      <c r="Y1122">
+        <v>12</v>
+      </c>
+      <c r="Z1122">
+        <v>78.2</v>
+      </c>
+      <c r="AA1122">
+        <v>11</v>
+      </c>
+      <c r="AB1122">
+        <v>75</v>
+      </c>
+      <c r="AC1122">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1123" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1123" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1123" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1123" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1123">
+        <v>100</v>
+      </c>
+      <c r="F1123">
+        <v>60.8</v>
+      </c>
+      <c r="G1123">
+        <v>24.8</v>
+      </c>
+      <c r="H1123">
+        <v>100</v>
+      </c>
+      <c r="I1123">
+        <v>100</v>
+      </c>
+      <c r="J1123">
+        <v>71.2</v>
+      </c>
+      <c r="K1123">
+        <v>11</v>
+      </c>
+      <c r="L1123">
+        <v>72.7</v>
+      </c>
+      <c r="M1123">
+        <v>13</v>
+      </c>
+      <c r="N1123">
+        <v>64.099999999999994</v>
+      </c>
+      <c r="O1123">
+        <v>19</v>
+      </c>
+      <c r="S1123"/>
+      <c r="T1123">
+        <v>58.7</v>
+      </c>
+      <c r="U1123">
+        <v>43</v>
+      </c>
+      <c r="V1123">
+        <v>69.3</v>
+      </c>
+      <c r="W1123">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1124" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1124" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1124" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1124" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1124">
+        <v>100</v>
+      </c>
+      <c r="F1124">
+        <v>66.3</v>
+      </c>
+      <c r="G1124">
+        <v>78.099999999999994</v>
+      </c>
+      <c r="H1124">
+        <v>0</v>
+      </c>
+      <c r="I1124">
+        <v>0</v>
+      </c>
+      <c r="J1124">
+        <v>65.900000000000006</v>
+      </c>
+      <c r="K1124">
+        <v>32</v>
+      </c>
+      <c r="L1124">
+        <v>67.8</v>
+      </c>
+      <c r="M1124">
+        <v>43</v>
+      </c>
+      <c r="N1124">
+        <v>81</v>
+      </c>
+      <c r="O1124">
+        <v>10</v>
+      </c>
+      <c r="P1124">
+        <v>74.2</v>
+      </c>
+      <c r="Q1124">
+        <v>16</v>
+      </c>
+      <c r="R1124">
+        <v>78.3</v>
+      </c>
+      <c r="S1124">
+        <v>11</v>
+      </c>
+      <c r="T1124">
+        <v>73.3</v>
+      </c>
+      <c r="U1124">
+        <v>24</v>
+      </c>
+      <c r="V1124">
+        <v>79.3</v>
+      </c>
+      <c r="W1124">
+        <v>14</v>
+      </c>
+      <c r="X1124">
+        <v>87.2</v>
+      </c>
+      <c r="Y1124">
+        <v>11</v>
+      </c>
+      <c r="Z1124">
+        <v>83.7</v>
+      </c>
+      <c r="AA1124">
+        <v>10</v>
+      </c>
+      <c r="AB1124">
+        <v>84.4</v>
+      </c>
+      <c r="AC1124">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1125" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1125" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1125" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1125" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1125">
+        <v>100</v>
+      </c>
+      <c r="F1125">
+        <v>62.5</v>
+      </c>
+      <c r="G1125">
+        <v>49.8</v>
+      </c>
+      <c r="H1125">
+        <v>100</v>
+      </c>
+      <c r="I1125">
+        <v>100</v>
+      </c>
+      <c r="J1125">
+        <v>62.5</v>
+      </c>
+      <c r="K1125">
+        <v>52</v>
+      </c>
+      <c r="L1125">
+        <v>67.099999999999994</v>
+      </c>
+      <c r="M1125">
+        <v>35</v>
+      </c>
+      <c r="N1125">
+        <v>70.900000000000006</v>
+      </c>
+      <c r="O1125">
+        <v>13</v>
+      </c>
+      <c r="P1125">
+        <v>65.8</v>
+      </c>
+      <c r="Q1125">
+        <v>18</v>
+      </c>
+      <c r="S1125"/>
+      <c r="T1125">
+        <v>69.099999999999994</v>
+      </c>
+      <c r="U1125">
+        <v>33</v>
+      </c>
+      <c r="V1125">
+        <v>83.7</v>
+      </c>
+      <c r="W1125">
+        <v>12</v>
+      </c>
+      <c r="X1125">
+        <v>81</v>
+      </c>
+      <c r="Y1125">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1126" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1126" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1126" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1126" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1126">
+        <v>99</v>
+      </c>
+      <c r="F1126">
+        <v>68.400000000000006</v>
+      </c>
+      <c r="G1126">
+        <v>86.3</v>
+      </c>
+      <c r="H1126">
+        <v>0</v>
+      </c>
+      <c r="I1126">
+        <v>0</v>
+      </c>
+      <c r="J1126">
+        <v>68.7</v>
+      </c>
+      <c r="K1126">
+        <v>32</v>
+      </c>
+      <c r="L1126">
+        <v>71.400000000000006</v>
+      </c>
+      <c r="M1126">
+        <v>41</v>
+      </c>
+      <c r="N1126">
+        <v>77.2</v>
+      </c>
+      <c r="O1126">
+        <v>12</v>
+      </c>
+      <c r="P1126">
+        <v>78.599999999999994</v>
+      </c>
+      <c r="Q1126">
+        <v>34</v>
+      </c>
+      <c r="R1126">
+        <v>86.5</v>
+      </c>
+      <c r="S1126">
+        <v>16</v>
+      </c>
+      <c r="T1126">
+        <v>75.400000000000006</v>
+      </c>
+      <c r="U1126">
+        <v>14</v>
+      </c>
+      <c r="V1126">
+        <v>82.4</v>
+      </c>
+      <c r="W1126">
+        <v>18</v>
+      </c>
+      <c r="X1126">
+        <v>84.9</v>
+      </c>
+      <c r="Y1126">
+        <v>11</v>
+      </c>
+      <c r="Z1126">
+        <v>85.7</v>
+      </c>
+      <c r="AA1126">
+        <v>12</v>
+      </c>
+      <c r="AB1126">
+        <v>83.3</v>
+      </c>
+      <c r="AC1126">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1127" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1127" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1127" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1127" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1127">
+        <v>100</v>
+      </c>
+      <c r="F1127">
+        <v>66.7</v>
+      </c>
+      <c r="G1127">
+        <v>100</v>
+      </c>
+      <c r="H1127">
+        <v>100</v>
+      </c>
+      <c r="I1127">
+        <v>100</v>
+      </c>
+      <c r="J1127">
+        <v>65.3</v>
+      </c>
+      <c r="K1127">
+        <v>61</v>
+      </c>
+      <c r="L1127">
+        <v>67.599999999999994</v>
+      </c>
+      <c r="M1127">
+        <v>40</v>
+      </c>
+      <c r="N1127">
+        <v>67.599999999999994</v>
+      </c>
+      <c r="O1127">
+        <v>14</v>
+      </c>
+      <c r="P1127">
+        <v>61.7</v>
+      </c>
+      <c r="Q1127">
+        <v>13</v>
+      </c>
+      <c r="R1127">
+        <v>63.4</v>
+      </c>
+      <c r="S1127">
+        <v>17</v>
+      </c>
+      <c r="T1127">
+        <v>69.900000000000006</v>
+      </c>
+      <c r="U1127">
+        <v>39</v>
+      </c>
+      <c r="V1127">
+        <v>73.7</v>
+      </c>
+      <c r="W1127">
+        <v>21</v>
+      </c>
+      <c r="X1127">
+        <v>73.900000000000006</v>
+      </c>
+      <c r="Y1127">
+        <v>10</v>
+      </c>
+      <c r="Z1127">
+        <v>74.599999999999994</v>
+      </c>
+      <c r="AA1127">
+        <v>12</v>
+      </c>
+      <c r="AB1127">
+        <v>73.900000000000006</v>
+      </c>
+      <c r="AC1127">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:AC1103" xr:uid="{3CACE78E-09B0-4A51-A9AF-2F3B2E4BAEFC}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AC1103">
+  <autoFilter ref="A1:AC1109" xr:uid="{3CACE78E-09B0-4A51-A9AF-2F3B2E4BAEFC}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AC1109">
       <sortCondition ref="A2:A97"/>
       <sortCondition ref="B2:B97"/>
       <sortCondition ref="C2:C97"/>

</xml_diff>

<commit_message>
poprawka do sortowania przy sklejaniu train i test
</commit_message>
<xml_diff>
--- a/wm/Results.xlsx
+++ b/wm/Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pioo\notebooks\wm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B0C5AA1-884A-45C6-883F-4BFBAA2D060D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FD58872-367D-4081-9570-1E922D2E8FFF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="690" yWindow="2640" windowWidth="26010" windowHeight="11385" tabRatio="435" xr2:uid="{B6B0453F-83A4-43EC-A328-DC10FEB5BD2E}"/>
+    <workbookView xWindow="240" yWindow="2745" windowWidth="28470" windowHeight="11340" tabRatio="435" xr2:uid="{B6B0453F-83A4-43EC-A328-DC10FEB5BD2E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3407" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3431" uniqueCount="84">
   <si>
     <t>Te_cal</t>
   </si>
@@ -278,6 +278,18 @@
   <si>
     <t>test23_16c</t>
   </si>
+  <si>
+    <t>test24_10c</t>
+  </si>
+  <si>
+    <t>test24_14c</t>
+  </si>
+  <si>
+    <t>test24_16c</t>
+  </si>
+  <si>
+    <t>test25_16c</t>
+  </si>
 </sst>
 </file>
 
@@ -334,7 +346,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -351,11 +363,60 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -365,6 +426,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -686,13 +752,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBA71D6A-A9B1-42AC-9396-7E4A540CDDDA}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:AC1127"/>
+  <dimension ref="A1:AC1135"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E1102" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E1109" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M1134" sqref="M1134"/>
+      <selection pane="bottomRight" activeCell="J1119" sqref="J1119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -85958,1397 +86024,1989 @@
         <v>10</v>
       </c>
     </row>
-    <row r="1110" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A1110" t="s">
+    <row r="1110" spans="1:29" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1110" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1110" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1110" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1110" s="10">
+        <v>100</v>
+      </c>
+      <c r="F1110" s="10">
+        <v>77.8</v>
+      </c>
+      <c r="G1110" s="10">
+        <v>98.6</v>
+      </c>
+      <c r="H1110" s="10">
+        <v>0</v>
+      </c>
+      <c r="I1110" s="10">
+        <v>0</v>
+      </c>
+      <c r="J1110" s="10">
+        <v>88.2</v>
+      </c>
+      <c r="K1110" s="10">
+        <v>24</v>
+      </c>
+      <c r="L1110" s="10">
+        <v>92.9</v>
+      </c>
+      <c r="M1110" s="10">
+        <v>19</v>
+      </c>
+      <c r="N1110" s="10">
+        <v>91.7</v>
+      </c>
+      <c r="O1110" s="10">
+        <v>17</v>
+      </c>
+      <c r="P1110" s="10">
+        <v>92.9</v>
+      </c>
+      <c r="Q1110" s="10">
+        <v>19</v>
+      </c>
+      <c r="R1110" s="10">
+        <v>94.7</v>
+      </c>
+      <c r="S1110" s="10">
+        <v>26</v>
+      </c>
+      <c r="T1110" s="10">
+        <v>91.7</v>
+      </c>
+      <c r="U1110" s="10">
+        <v>17</v>
+      </c>
+      <c r="V1110" s="10">
+        <v>100</v>
+      </c>
+      <c r="W1110" s="10">
+        <v>10</v>
+      </c>
+      <c r="X1110" s="10">
+        <v>100</v>
+      </c>
+      <c r="Y1110" s="10">
+        <v>14</v>
+      </c>
+      <c r="Z1110" s="10">
+        <v>100</v>
+      </c>
+      <c r="AA1110" s="10">
+        <v>10</v>
+      </c>
+      <c r="AB1110" s="10">
+        <v>100</v>
+      </c>
+      <c r="AC1110" s="10">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1111" spans="1:29" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1111" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1111" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1111" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1111" s="7">
+        <v>100</v>
+      </c>
+      <c r="F1111" s="7">
+        <v>69.400000000000006</v>
+      </c>
+      <c r="G1111" s="7">
+        <v>4.2</v>
+      </c>
+      <c r="H1111" s="7">
+        <v>100</v>
+      </c>
+      <c r="I1111" s="7">
+        <v>100</v>
+      </c>
+      <c r="J1111" s="7">
+        <v>100</v>
+      </c>
+      <c r="K1111" s="7">
+        <v>10</v>
+      </c>
+      <c r="L1111" s="7">
+        <v>100</v>
+      </c>
+      <c r="M1111" s="7">
+        <v>11</v>
+      </c>
+      <c r="T1111" s="7">
+        <v>72</v>
+      </c>
+      <c r="U1111" s="7">
+        <v>35</v>
+      </c>
+      <c r="V1111" s="7">
+        <v>87.5</v>
+      </c>
+      <c r="W1111" s="7">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1112" spans="1:29" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1112" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1112" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1112" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1112" s="7">
+        <v>100</v>
+      </c>
+      <c r="F1112" s="7">
+        <v>83.3</v>
+      </c>
+      <c r="G1112" s="7">
+        <v>98.3</v>
+      </c>
+      <c r="H1112" s="7">
+        <v>0</v>
+      </c>
+      <c r="I1112" s="7">
+        <v>0</v>
+      </c>
+      <c r="J1112" s="7">
+        <v>100</v>
+      </c>
+      <c r="K1112" s="7">
+        <v>17</v>
+      </c>
+      <c r="L1112" s="7">
+        <v>100</v>
+      </c>
+      <c r="M1112" s="7">
+        <v>17</v>
+      </c>
+      <c r="N1112" s="7">
+        <v>100</v>
+      </c>
+      <c r="O1112" s="7">
+        <v>17</v>
+      </c>
+      <c r="P1112" s="7">
+        <v>100</v>
+      </c>
+      <c r="Q1112" s="7">
+        <v>17</v>
+      </c>
+      <c r="R1112" s="7">
+        <v>100</v>
+      </c>
+      <c r="S1112" s="7">
+        <v>17</v>
+      </c>
+      <c r="T1112" s="7">
+        <v>88.2</v>
+      </c>
+      <c r="U1112" s="7">
+        <v>28</v>
+      </c>
+      <c r="V1112" s="7">
+        <v>92.3</v>
+      </c>
+      <c r="W1112" s="7">
+        <v>22</v>
+      </c>
+      <c r="X1112" s="7">
+        <v>100</v>
+      </c>
+      <c r="Y1112" s="7">
+        <v>10</v>
+      </c>
+      <c r="Z1112" s="7">
+        <v>90.9</v>
+      </c>
+      <c r="AA1112" s="7">
+        <v>18</v>
+      </c>
+      <c r="AB1112" s="7">
+        <v>92.9</v>
+      </c>
+      <c r="AC1112" s="7">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="1113" spans="1:29" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1113" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1113" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1113" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1113" s="7">
+        <v>100</v>
+      </c>
+      <c r="F1113" s="7">
+        <v>76.7</v>
+      </c>
+      <c r="G1113" s="7">
+        <v>33.299999999999997</v>
+      </c>
+      <c r="H1113" s="7">
+        <v>100</v>
+      </c>
+      <c r="I1113" s="7">
+        <v>100</v>
+      </c>
+      <c r="J1113" s="7">
+        <v>77.3</v>
+      </c>
+      <c r="K1113" s="7">
+        <v>37</v>
+      </c>
+      <c r="L1113" s="7">
+        <v>100</v>
+      </c>
+      <c r="M1113" s="7">
+        <v>10</v>
+      </c>
+      <c r="N1113" s="7">
+        <v>100</v>
+      </c>
+      <c r="O1113" s="7">
+        <v>13</v>
+      </c>
+      <c r="T1113" s="7">
+        <v>87.5</v>
+      </c>
+      <c r="U1113" s="7">
+        <v>40</v>
+      </c>
+      <c r="V1113" s="7">
+        <v>91.7</v>
+      </c>
+      <c r="W1113" s="7">
+        <v>20</v>
+      </c>
+      <c r="X1113" s="7">
+        <v>87.5</v>
+      </c>
+      <c r="Y1113" s="7">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1114" spans="1:29" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1114" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1114" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1114" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1114" s="7">
+        <v>98.4</v>
+      </c>
+      <c r="F1114" s="7">
+        <v>80.3</v>
+      </c>
+      <c r="G1114" s="7">
+        <v>97</v>
+      </c>
+      <c r="H1114" s="7">
+        <v>0</v>
+      </c>
+      <c r="I1114" s="7">
+        <v>0</v>
+      </c>
+      <c r="J1114" s="7">
+        <v>100</v>
+      </c>
+      <c r="K1114" s="7">
+        <v>24</v>
+      </c>
+      <c r="L1114" s="7">
+        <v>100</v>
+      </c>
+      <c r="M1114" s="7">
+        <v>23</v>
+      </c>
+      <c r="N1114" s="7">
+        <v>100</v>
+      </c>
+      <c r="O1114" s="7">
+        <v>20</v>
+      </c>
+      <c r="P1114" s="7">
+        <v>100</v>
+      </c>
+      <c r="Q1114" s="7">
+        <v>14</v>
+      </c>
+      <c r="R1114" s="7">
+        <v>100</v>
+      </c>
+      <c r="S1114" s="7">
+        <v>14</v>
+      </c>
+      <c r="T1114" s="7">
+        <v>85.7</v>
+      </c>
+      <c r="U1114" s="7">
+        <v>21</v>
+      </c>
+      <c r="V1114" s="7">
+        <v>87.5</v>
+      </c>
+      <c r="W1114" s="7">
+        <v>12</v>
+      </c>
+      <c r="X1114" s="7">
+        <v>87.5</v>
+      </c>
+      <c r="Y1114" s="7">
+        <v>12</v>
+      </c>
+      <c r="Z1114" s="7">
+        <v>90</v>
+      </c>
+      <c r="AA1114" s="7">
+        <v>15</v>
+      </c>
+      <c r="AB1114" s="7">
+        <v>100</v>
+      </c>
+      <c r="AC1114" s="7">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1115" spans="1:29" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1115" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1115" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1115" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1115" s="13">
+        <v>100</v>
+      </c>
+      <c r="F1115" s="13">
+        <v>77.3</v>
+      </c>
+      <c r="G1115" s="13">
+        <v>69.7</v>
+      </c>
+      <c r="H1115" s="13">
+        <v>100</v>
+      </c>
+      <c r="I1115" s="13">
+        <v>100</v>
+      </c>
+      <c r="J1115" s="13">
+        <v>100</v>
+      </c>
+      <c r="K1115" s="13">
+        <v>12</v>
+      </c>
+      <c r="L1115" s="13">
+        <v>100</v>
+      </c>
+      <c r="M1115" s="13">
+        <v>24</v>
+      </c>
+      <c r="N1115" s="13">
+        <v>100</v>
+      </c>
+      <c r="O1115" s="13">
+        <v>11</v>
+      </c>
+      <c r="P1115" s="13">
+        <v>100</v>
+      </c>
+      <c r="Q1115" s="13">
+        <v>11</v>
+      </c>
+      <c r="R1115" s="13">
+        <v>71.400000000000006</v>
+      </c>
+      <c r="S1115" s="13">
+        <v>11</v>
+      </c>
+      <c r="T1115" s="13">
+        <v>71.400000000000006</v>
+      </c>
+      <c r="U1115" s="13">
+        <v>21</v>
+      </c>
+      <c r="V1115" s="13">
+        <v>80</v>
+      </c>
+      <c r="W1115" s="13">
+        <v>23</v>
+      </c>
+      <c r="X1115" s="13">
+        <v>88.9</v>
+      </c>
+      <c r="Y1115" s="13">
+        <v>14</v>
+      </c>
+      <c r="Z1115" s="13">
+        <v>88.9</v>
+      </c>
+      <c r="AA1115" s="13">
+        <v>14</v>
+      </c>
+      <c r="AB1115" s="13">
+        <v>85.7</v>
+      </c>
+      <c r="AC1115" s="13">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1116" spans="1:29" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1116" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="B1110" t="s">
+      <c r="B1116" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="D1110" t="s">
+      <c r="D1116" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="E1110">
-        <v>100</v>
-      </c>
-      <c r="F1110">
+      <c r="E1116" s="10">
+        <v>100</v>
+      </c>
+      <c r="F1116" s="10">
         <v>65.599999999999994</v>
       </c>
-      <c r="G1110">
+      <c r="G1116" s="10">
         <v>85.4</v>
       </c>
-      <c r="H1110">
+      <c r="H1116" s="10">
         <v>0</v>
       </c>
-      <c r="I1110">
+      <c r="I1116" s="10">
         <v>0</v>
       </c>
-      <c r="J1110">
+      <c r="J1116" s="10">
         <v>67.400000000000006</v>
       </c>
-      <c r="K1110">
+      <c r="K1116" s="10">
         <v>43</v>
       </c>
-      <c r="L1110">
+      <c r="L1116" s="10">
         <v>78.900000000000006</v>
       </c>
-      <c r="M1110">
+      <c r="M1116" s="10">
         <v>12</v>
       </c>
-      <c r="N1110">
+      <c r="N1116" s="10">
         <v>84.8</v>
       </c>
-      <c r="O1110">
+      <c r="O1116" s="10">
         <v>11</v>
       </c>
-      <c r="P1110">
+      <c r="P1116" s="10">
         <v>83.9</v>
       </c>
-      <c r="Q1110">
-        <v>10</v>
-      </c>
-      <c r="R1110">
+      <c r="Q1116" s="10">
+        <v>10</v>
+      </c>
+      <c r="R1116" s="10">
         <v>87.9</v>
       </c>
-      <c r="S1110">
+      <c r="S1116" s="10">
         <v>11</v>
       </c>
-      <c r="T1110">
+      <c r="T1116" s="10">
         <v>75.599999999999994</v>
       </c>
-      <c r="U1110">
+      <c r="U1116" s="10">
         <v>27</v>
       </c>
-      <c r="V1110">
+      <c r="V1116" s="10">
         <v>80.5</v>
       </c>
-      <c r="W1110">
+      <c r="W1116" s="10">
         <v>13</v>
       </c>
-      <c r="X1110">
+      <c r="X1116" s="10">
         <v>87.1</v>
       </c>
-      <c r="Y1110">
-        <v>10</v>
-      </c>
-      <c r="Z1110">
+      <c r="Y1116" s="10">
+        <v>10</v>
+      </c>
+      <c r="Z1116" s="10">
         <v>84.4</v>
       </c>
-      <c r="AA1110">
-        <v>10</v>
-      </c>
-      <c r="AB1110">
+      <c r="AA1116" s="10">
+        <v>10</v>
+      </c>
+      <c r="AB1116" s="10">
         <v>84.4</v>
       </c>
-      <c r="AC1110">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="1111" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A1111" t="s">
+      <c r="AC1116" s="10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1117" spans="1:29" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1117" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="B1111" t="s">
+      <c r="B1117" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D1111" t="s">
+      <c r="D1117" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="E1111">
-        <v>100</v>
-      </c>
-      <c r="F1111">
+      <c r="E1117" s="7">
+        <v>100</v>
+      </c>
+      <c r="F1117" s="7">
         <v>61.8</v>
       </c>
-      <c r="G1111">
+      <c r="G1117" s="7">
         <v>25.5</v>
       </c>
-      <c r="H1111">
-        <v>100</v>
-      </c>
-      <c r="I1111">
-        <v>100</v>
-      </c>
-      <c r="J1111">
+      <c r="H1117" s="7">
+        <v>100</v>
+      </c>
+      <c r="I1117" s="7">
+        <v>100</v>
+      </c>
+      <c r="J1117" s="7">
         <v>74</v>
       </c>
-      <c r="K1111">
+      <c r="K1117" s="7">
         <v>16</v>
       </c>
-      <c r="L1111">
+      <c r="L1117" s="7">
         <v>72</v>
       </c>
-      <c r="M1111">
+      <c r="M1117" s="7">
         <v>16</v>
       </c>
-      <c r="N1111">
+      <c r="N1117" s="7">
         <v>81.8</v>
       </c>
-      <c r="O1111">
+      <c r="O1117" s="7">
         <v>11</v>
       </c>
-      <c r="S1111"/>
-      <c r="T1111">
+      <c r="T1117" s="7">
         <v>61.3</v>
       </c>
-      <c r="U1111">
+      <c r="U1117" s="7">
         <v>45</v>
       </c>
-      <c r="V1111">
+      <c r="V1117" s="7">
         <v>76.3</v>
       </c>
-      <c r="W1111">
+      <c r="W1117" s="7">
         <v>19</v>
       </c>
-      <c r="X1111">
+      <c r="X1117" s="7">
         <v>80.599999999999994</v>
       </c>
-      <c r="Y1111">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="1112" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A1112" t="s">
+      <c r="Y1117" s="7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1118" spans="1:29" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1118" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="B1112" t="s">
+      <c r="B1118" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D1112" t="s">
+      <c r="D1118" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="E1112">
-        <v>100</v>
-      </c>
-      <c r="F1112">
+      <c r="E1118" s="7">
+        <v>100</v>
+      </c>
+      <c r="F1118" s="7">
         <v>67.8</v>
       </c>
-      <c r="G1112">
+      <c r="G1118" s="7">
         <v>79.8</v>
       </c>
-      <c r="H1112">
+      <c r="H1118" s="7">
         <v>0</v>
       </c>
-      <c r="I1112">
+      <c r="I1118" s="7">
         <v>0</v>
       </c>
-      <c r="J1112">
+      <c r="J1118" s="7">
         <v>66</v>
       </c>
-      <c r="K1112">
+      <c r="K1118" s="7">
         <v>54</v>
       </c>
-      <c r="L1112">
+      <c r="L1118" s="7">
         <v>71.900000000000006</v>
       </c>
-      <c r="M1112">
+      <c r="M1118" s="7">
         <v>33</v>
       </c>
-      <c r="N1112">
+      <c r="N1118" s="7">
         <v>77</v>
       </c>
-      <c r="O1112">
+      <c r="O1118" s="7">
         <v>23</v>
       </c>
-      <c r="P1112">
+      <c r="P1118" s="7">
         <v>85.7</v>
       </c>
-      <c r="Q1112">
-        <v>10</v>
-      </c>
-      <c r="R1112">
+      <c r="Q1118" s="7">
+        <v>10</v>
+      </c>
+      <c r="R1118" s="7">
         <v>88.5</v>
       </c>
-      <c r="S1112">
-        <v>10</v>
-      </c>
-      <c r="T1112">
+      <c r="S1118" s="7">
+        <v>10</v>
+      </c>
+      <c r="T1118" s="7">
         <v>76.7</v>
       </c>
-      <c r="U1112">
+      <c r="U1118" s="7">
         <v>22</v>
       </c>
-      <c r="V1112">
+      <c r="V1118" s="7">
         <v>87.1</v>
       </c>
-      <c r="W1112">
+      <c r="W1118" s="7">
         <v>12</v>
       </c>
-      <c r="X1112">
+      <c r="X1118" s="7">
         <v>89.3</v>
       </c>
-      <c r="Y1112">
-        <v>10</v>
-      </c>
-      <c r="Z1112">
+      <c r="Y1118" s="7">
+        <v>10</v>
+      </c>
+      <c r="Z1118" s="7">
         <v>82.1</v>
       </c>
-      <c r="AA1112">
-        <v>10</v>
-      </c>
-      <c r="AB1112">
+      <c r="AA1118" s="7">
+        <v>10</v>
+      </c>
+      <c r="AB1118" s="7">
         <v>83.9</v>
       </c>
-      <c r="AC1112">
+      <c r="AC1118" s="7">
         <v>12</v>
       </c>
     </row>
-    <row r="1113" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A1113" t="s">
+    <row r="1119" spans="1:29" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1119" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="B1113" t="s">
+      <c r="B1119" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D1113" t="s">
+      <c r="D1119" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="E1113">
-        <v>100</v>
-      </c>
-      <c r="F1113">
+      <c r="E1119" s="7">
+        <v>100</v>
+      </c>
+      <c r="F1119" s="7">
         <v>65.900000000000006</v>
       </c>
-      <c r="G1113">
+      <c r="G1119" s="7">
         <v>27</v>
       </c>
-      <c r="H1113">
-        <v>100</v>
-      </c>
-      <c r="I1113">
-        <v>100</v>
-      </c>
-      <c r="J1113">
+      <c r="H1119" s="7">
+        <v>100</v>
+      </c>
+      <c r="I1119" s="7">
+        <v>100</v>
+      </c>
+      <c r="J1119" s="7">
         <v>66.3</v>
       </c>
-      <c r="K1113">
+      <c r="K1119" s="7">
         <v>37</v>
       </c>
-      <c r="L1113">
+      <c r="L1119" s="7">
         <v>71.8</v>
       </c>
-      <c r="M1113">
+      <c r="M1119" s="7">
         <v>32</v>
       </c>
-      <c r="N1113">
+      <c r="N1119" s="7">
         <v>85.7</v>
       </c>
-      <c r="O1113">
+      <c r="O1119" s="7">
         <v>13</v>
       </c>
-      <c r="S1113"/>
-      <c r="T1113">
+      <c r="T1119" s="7">
         <v>69.3</v>
       </c>
-      <c r="U1113">
+      <c r="U1119" s="7">
         <v>38</v>
       </c>
-      <c r="V1113">
+      <c r="V1119" s="7">
         <v>83.8</v>
       </c>
-      <c r="W1113">
+      <c r="W1119" s="7">
         <v>14</v>
       </c>
-      <c r="X1113">
+      <c r="X1119" s="7">
         <v>66.7</v>
       </c>
-      <c r="Y1113">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="1114" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A1114" t="s">
+      <c r="Y1119" s="7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1120" spans="1:29" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1120" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="B1114" t="s">
+      <c r="B1120" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D1114" t="s">
+      <c r="D1120" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="E1114">
+      <c r="E1120" s="7">
         <v>99.2</v>
       </c>
-      <c r="F1114">
+      <c r="F1120" s="7">
         <v>66.7</v>
       </c>
-      <c r="G1114">
+      <c r="G1120" s="7">
         <v>80.2</v>
       </c>
-      <c r="H1114">
+      <c r="H1120" s="7">
         <v>0</v>
       </c>
-      <c r="I1114">
+      <c r="I1120" s="7">
         <v>0</v>
       </c>
-      <c r="J1114">
+      <c r="J1120" s="7">
         <v>72.400000000000006</v>
       </c>
-      <c r="K1114">
+      <c r="K1120" s="7">
         <v>38</v>
       </c>
-      <c r="L1114">
+      <c r="L1120" s="7">
         <v>78.3</v>
       </c>
-      <c r="M1114">
+      <c r="M1120" s="7">
         <v>27</v>
       </c>
-      <c r="N1114">
+      <c r="N1120" s="7">
         <v>90.9</v>
       </c>
-      <c r="O1114">
+      <c r="O1120" s="7">
         <v>11</v>
       </c>
-      <c r="P1114">
+      <c r="P1120" s="7">
         <v>88.6</v>
       </c>
-      <c r="Q1114">
+      <c r="Q1120" s="7">
         <v>12</v>
       </c>
-      <c r="R1114">
+      <c r="R1120" s="7">
         <v>90</v>
       </c>
-      <c r="S1114">
-        <v>10</v>
-      </c>
-      <c r="T1114">
+      <c r="S1120" s="7">
+        <v>10</v>
+      </c>
+      <c r="T1120" s="7">
         <v>75</v>
       </c>
-      <c r="U1114">
+      <c r="U1120" s="7">
         <v>13</v>
       </c>
-      <c r="V1114">
+      <c r="V1120" s="7">
         <v>86.7</v>
       </c>
-      <c r="W1114">
-        <v>10</v>
-      </c>
-      <c r="X1114">
+      <c r="W1120" s="7">
+        <v>10</v>
+      </c>
+      <c r="X1120" s="7">
         <v>85.7</v>
       </c>
-      <c r="Y1114">
+      <c r="Y1120" s="7">
         <v>16</v>
       </c>
-      <c r="Z1114">
+      <c r="Z1120" s="7">
         <v>87.1</v>
       </c>
-      <c r="AA1114">
-        <v>10</v>
-      </c>
-      <c r="AB1114">
+      <c r="AA1120" s="7">
+        <v>10</v>
+      </c>
+      <c r="AB1120" s="7">
         <v>86.8</v>
       </c>
-      <c r="AC1114">
+      <c r="AC1120" s="7">
         <v>13</v>
       </c>
     </row>
-    <row r="1115" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A1115" t="s">
+    <row r="1121" spans="1:29" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1121" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="B1115" t="s">
+      <c r="B1121" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="D1115" t="s">
+      <c r="D1121" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="E1115">
-        <v>100</v>
-      </c>
-      <c r="F1115">
+      <c r="E1121" s="13">
+        <v>100</v>
+      </c>
+      <c r="F1121" s="13">
         <v>64.7</v>
       </c>
-      <c r="G1115">
+      <c r="G1121" s="13">
         <v>60.7</v>
       </c>
-      <c r="H1115">
-        <v>100</v>
-      </c>
-      <c r="I1115">
-        <v>100</v>
-      </c>
-      <c r="J1115">
+      <c r="H1121" s="13">
+        <v>100</v>
+      </c>
+      <c r="I1121" s="13">
+        <v>100</v>
+      </c>
+      <c r="J1121" s="13">
         <v>68</v>
       </c>
-      <c r="K1115">
+      <c r="K1121" s="13">
         <v>40</v>
       </c>
-      <c r="L1115">
+      <c r="L1121" s="13">
         <v>86.7</v>
       </c>
-      <c r="M1115">
+      <c r="M1121" s="13">
         <v>20</v>
       </c>
-      <c r="N1115">
+      <c r="N1121" s="13">
         <v>82.8</v>
       </c>
-      <c r="O1115">
-        <v>10</v>
-      </c>
-      <c r="P1115">
+      <c r="O1121" s="13">
+        <v>10</v>
+      </c>
+      <c r="P1121" s="13">
         <v>67.3</v>
       </c>
-      <c r="Q1115">
+      <c r="Q1121" s="13">
         <v>17</v>
       </c>
-      <c r="S1115"/>
-      <c r="T1115">
+      <c r="T1121" s="13">
         <v>65.5</v>
       </c>
-      <c r="U1115">
+      <c r="U1121" s="13">
         <v>36</v>
       </c>
-      <c r="V1115">
+      <c r="V1121" s="13">
         <v>76.7</v>
       </c>
-      <c r="W1115">
-        <v>10</v>
-      </c>
-      <c r="X1115">
+      <c r="W1121" s="13">
+        <v>10</v>
+      </c>
+      <c r="X1121" s="13">
         <v>79.5</v>
       </c>
-      <c r="Y1115">
+      <c r="Y1121" s="13">
         <v>13</v>
       </c>
-      <c r="Z1115">
+      <c r="Z1121" s="13">
         <v>78.8</v>
       </c>
-      <c r="AA1115">
+      <c r="AA1121" s="13">
         <v>11</v>
       </c>
-      <c r="AB1115">
+      <c r="AB1121" s="13">
         <v>66.7</v>
       </c>
-      <c r="AC1115">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="1116" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A1116" t="s">
-        <v>74</v>
-      </c>
-      <c r="B1116" t="s">
+      <c r="AC1121" s="13">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1122" spans="1:29" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1122" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1122" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="D1116" t="s">
+      <c r="D1122" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="E1116">
-        <v>100</v>
-      </c>
-      <c r="F1116">
-        <v>77.8</v>
-      </c>
-      <c r="G1116">
-        <v>98.6</v>
-      </c>
-      <c r="H1116">
+      <c r="E1122" s="10">
+        <v>100</v>
+      </c>
+      <c r="F1122" s="10">
+        <v>61.4</v>
+      </c>
+      <c r="G1122" s="10">
+        <v>82.2</v>
+      </c>
+      <c r="H1122" s="10">
         <v>0</v>
       </c>
-      <c r="I1116">
+      <c r="I1122" s="10">
         <v>0</v>
       </c>
-      <c r="J1116">
-        <v>88.2</v>
-      </c>
-      <c r="K1116">
+      <c r="J1122" s="10">
+        <v>69.599999999999994</v>
+      </c>
+      <c r="K1122" s="10">
+        <v>19</v>
+      </c>
+      <c r="L1122" s="10">
+        <v>74.5</v>
+      </c>
+      <c r="M1122" s="10">
+        <v>10</v>
+      </c>
+      <c r="N1122" s="10">
+        <v>73.8</v>
+      </c>
+      <c r="O1122" s="10">
+        <v>16</v>
+      </c>
+      <c r="P1122" s="10">
+        <v>78.8</v>
+      </c>
+      <c r="Q1122" s="10">
+        <v>11</v>
+      </c>
+      <c r="R1122" s="10">
+        <v>73.099999999999994</v>
+      </c>
+      <c r="S1122" s="10">
+        <v>11</v>
+      </c>
+      <c r="T1122" s="10">
+        <v>69.2</v>
+      </c>
+      <c r="U1122" s="10">
+        <v>16</v>
+      </c>
+      <c r="V1122" s="10">
+        <v>74.5</v>
+      </c>
+      <c r="W1122" s="10">
+        <v>11</v>
+      </c>
+      <c r="X1122" s="10">
+        <v>78</v>
+      </c>
+      <c r="Y1122" s="10">
+        <v>12</v>
+      </c>
+      <c r="Z1122" s="10">
+        <v>78.2</v>
+      </c>
+      <c r="AA1122" s="10">
+        <v>11</v>
+      </c>
+      <c r="AB1122" s="10">
+        <v>75</v>
+      </c>
+      <c r="AC1122" s="10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1123" spans="1:29" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1123" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1123" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1123" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1123" s="7">
+        <v>100</v>
+      </c>
+      <c r="F1123" s="7">
+        <v>60.8</v>
+      </c>
+      <c r="G1123" s="7">
+        <v>24.8</v>
+      </c>
+      <c r="H1123" s="7">
+        <v>100</v>
+      </c>
+      <c r="I1123" s="7">
+        <v>100</v>
+      </c>
+      <c r="J1123" s="7">
+        <v>71.2</v>
+      </c>
+      <c r="K1123" s="7">
+        <v>11</v>
+      </c>
+      <c r="L1123" s="7">
+        <v>72.7</v>
+      </c>
+      <c r="M1123" s="7">
+        <v>13</v>
+      </c>
+      <c r="N1123" s="7">
+        <v>64.099999999999994</v>
+      </c>
+      <c r="O1123" s="7">
+        <v>19</v>
+      </c>
+      <c r="T1123" s="7">
+        <v>58.7</v>
+      </c>
+      <c r="U1123" s="7">
+        <v>43</v>
+      </c>
+      <c r="V1123" s="7">
+        <v>69.3</v>
+      </c>
+      <c r="W1123" s="7">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1124" spans="1:29" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1124" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1124" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1124" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1124" s="7">
+        <v>100</v>
+      </c>
+      <c r="F1124" s="7">
+        <v>66.3</v>
+      </c>
+      <c r="G1124" s="7">
+        <v>78.099999999999994</v>
+      </c>
+      <c r="H1124" s="7">
+        <v>0</v>
+      </c>
+      <c r="I1124" s="7">
+        <v>0</v>
+      </c>
+      <c r="J1124" s="7">
+        <v>65.900000000000006</v>
+      </c>
+      <c r="K1124" s="7">
+        <v>32</v>
+      </c>
+      <c r="L1124" s="7">
+        <v>67.8</v>
+      </c>
+      <c r="M1124" s="7">
+        <v>43</v>
+      </c>
+      <c r="N1124" s="7">
+        <v>81</v>
+      </c>
+      <c r="O1124" s="7">
+        <v>10</v>
+      </c>
+      <c r="P1124" s="7">
+        <v>74.2</v>
+      </c>
+      <c r="Q1124" s="7">
+        <v>16</v>
+      </c>
+      <c r="R1124" s="7">
+        <v>78.3</v>
+      </c>
+      <c r="S1124" s="7">
+        <v>11</v>
+      </c>
+      <c r="T1124" s="7">
+        <v>73.3</v>
+      </c>
+      <c r="U1124" s="7">
         <v>24</v>
       </c>
-      <c r="L1116">
+      <c r="V1124" s="7">
+        <v>79.3</v>
+      </c>
+      <c r="W1124" s="7">
+        <v>14</v>
+      </c>
+      <c r="X1124" s="7">
+        <v>87.2</v>
+      </c>
+      <c r="Y1124" s="7">
+        <v>11</v>
+      </c>
+      <c r="Z1124" s="7">
+        <v>83.7</v>
+      </c>
+      <c r="AA1124" s="7">
+        <v>10</v>
+      </c>
+      <c r="AB1124" s="7">
+        <v>84.4</v>
+      </c>
+      <c r="AC1124" s="7">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1125" spans="1:29" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1125" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1125" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1125" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1125" s="7">
+        <v>100</v>
+      </c>
+      <c r="F1125" s="7">
+        <v>62.5</v>
+      </c>
+      <c r="G1125" s="7">
+        <v>49.8</v>
+      </c>
+      <c r="H1125" s="7">
+        <v>100</v>
+      </c>
+      <c r="I1125" s="7">
+        <v>100</v>
+      </c>
+      <c r="J1125" s="7">
+        <v>62.5</v>
+      </c>
+      <c r="K1125" s="7">
+        <v>52</v>
+      </c>
+      <c r="L1125" s="7">
+        <v>67.099999999999994</v>
+      </c>
+      <c r="M1125" s="7">
+        <v>35</v>
+      </c>
+      <c r="N1125" s="7">
+        <v>70.900000000000006</v>
+      </c>
+      <c r="O1125" s="7">
+        <v>13</v>
+      </c>
+      <c r="P1125" s="7">
+        <v>65.8</v>
+      </c>
+      <c r="Q1125" s="7">
+        <v>18</v>
+      </c>
+      <c r="T1125" s="7">
+        <v>69.099999999999994</v>
+      </c>
+      <c r="U1125" s="7">
+        <v>33</v>
+      </c>
+      <c r="V1125" s="7">
+        <v>83.7</v>
+      </c>
+      <c r="W1125" s="7">
+        <v>12</v>
+      </c>
+      <c r="X1125" s="7">
+        <v>81</v>
+      </c>
+      <c r="Y1125" s="7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1126" spans="1:29" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1126" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1126" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1126" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1126" s="7">
+        <v>99</v>
+      </c>
+      <c r="F1126" s="7">
+        <v>68.400000000000006</v>
+      </c>
+      <c r="G1126" s="7">
+        <v>86.3</v>
+      </c>
+      <c r="H1126" s="7">
+        <v>0</v>
+      </c>
+      <c r="I1126" s="7">
+        <v>0</v>
+      </c>
+      <c r="J1126" s="7">
+        <v>68.7</v>
+      </c>
+      <c r="K1126" s="7">
+        <v>32</v>
+      </c>
+      <c r="L1126" s="7">
+        <v>71.400000000000006</v>
+      </c>
+      <c r="M1126" s="7">
+        <v>41</v>
+      </c>
+      <c r="N1126" s="7">
+        <v>77.2</v>
+      </c>
+      <c r="O1126" s="7">
+        <v>12</v>
+      </c>
+      <c r="P1126" s="7">
+        <v>78.599999999999994</v>
+      </c>
+      <c r="Q1126" s="7">
+        <v>34</v>
+      </c>
+      <c r="R1126" s="7">
+        <v>86.5</v>
+      </c>
+      <c r="S1126" s="7">
+        <v>16</v>
+      </c>
+      <c r="T1126" s="7">
+        <v>75.400000000000006</v>
+      </c>
+      <c r="U1126" s="7">
+        <v>14</v>
+      </c>
+      <c r="V1126" s="7">
+        <v>82.4</v>
+      </c>
+      <c r="W1126" s="7">
+        <v>18</v>
+      </c>
+      <c r="X1126" s="7">
+        <v>84.9</v>
+      </c>
+      <c r="Y1126" s="7">
+        <v>11</v>
+      </c>
+      <c r="Z1126" s="7">
+        <v>85.7</v>
+      </c>
+      <c r="AA1126" s="7">
+        <v>12</v>
+      </c>
+      <c r="AB1126" s="7">
+        <v>83.3</v>
+      </c>
+      <c r="AC1126" s="7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1127" spans="1:29" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1127" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1127" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1127" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1127" s="13">
+        <v>100</v>
+      </c>
+      <c r="F1127" s="13">
+        <v>66.7</v>
+      </c>
+      <c r="G1127" s="13">
+        <v>100</v>
+      </c>
+      <c r="H1127" s="13">
+        <v>100</v>
+      </c>
+      <c r="I1127" s="13">
+        <v>100</v>
+      </c>
+      <c r="J1127" s="13">
+        <v>65.3</v>
+      </c>
+      <c r="K1127" s="13">
+        <v>61</v>
+      </c>
+      <c r="L1127" s="13">
+        <v>67.599999999999994</v>
+      </c>
+      <c r="M1127" s="13">
+        <v>40</v>
+      </c>
+      <c r="N1127" s="13">
+        <v>67.599999999999994</v>
+      </c>
+      <c r="O1127" s="13">
+        <v>14</v>
+      </c>
+      <c r="P1127" s="13">
+        <v>61.7</v>
+      </c>
+      <c r="Q1127" s="13">
+        <v>13</v>
+      </c>
+      <c r="R1127" s="13">
+        <v>63.4</v>
+      </c>
+      <c r="S1127" s="13">
+        <v>17</v>
+      </c>
+      <c r="T1127" s="13">
+        <v>69.900000000000006</v>
+      </c>
+      <c r="U1127" s="13">
+        <v>39</v>
+      </c>
+      <c r="V1127" s="13">
+        <v>73.7</v>
+      </c>
+      <c r="W1127" s="13">
+        <v>21</v>
+      </c>
+      <c r="X1127" s="13">
+        <v>73.900000000000006</v>
+      </c>
+      <c r="Y1127" s="13">
+        <v>10</v>
+      </c>
+      <c r="Z1127" s="13">
+        <v>74.599999999999994</v>
+      </c>
+      <c r="AA1127" s="13">
+        <v>12</v>
+      </c>
+      <c r="AB1127" s="13">
+        <v>73.900000000000006</v>
+      </c>
+      <c r="AC1127" s="13">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1128" spans="1:29" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1128" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1128" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1128" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1128" s="10">
+        <v>100</v>
+      </c>
+      <c r="F1128" s="10">
+        <v>69.2</v>
+      </c>
+      <c r="G1128" s="10">
+        <v>86.3</v>
+      </c>
+      <c r="H1128" s="10">
+        <v>0</v>
+      </c>
+      <c r="I1128" s="10">
+        <v>0</v>
+      </c>
+      <c r="J1128" s="10">
+        <v>81.8</v>
+      </c>
+      <c r="K1128" s="10">
+        <v>17</v>
+      </c>
+      <c r="L1128" s="10">
+        <v>84.4</v>
+      </c>
+      <c r="M1128" s="10">
+        <v>24</v>
+      </c>
+      <c r="N1128" s="10">
+        <v>90.3</v>
+      </c>
+      <c r="O1128" s="10">
+        <v>12</v>
+      </c>
+      <c r="P1128" s="10">
+        <v>94.6</v>
+      </c>
+      <c r="Q1128" s="10">
+        <v>14</v>
+      </c>
+      <c r="R1128" s="10">
+        <v>96</v>
+      </c>
+      <c r="S1128" s="10">
+        <v>10</v>
+      </c>
+      <c r="T1128" s="10">
+        <v>67.8</v>
+      </c>
+      <c r="U1128" s="10">
+        <v>34</v>
+      </c>
+      <c r="V1128" s="10">
+        <v>78.8</v>
+      </c>
+      <c r="W1128" s="10">
+        <v>13</v>
+      </c>
+      <c r="X1128" s="10">
+        <v>82.1</v>
+      </c>
+      <c r="Y1128" s="10">
+        <v>11</v>
+      </c>
+      <c r="Z1128" s="10">
+        <v>92</v>
+      </c>
+      <c r="AA1128" s="10">
+        <v>10</v>
+      </c>
+      <c r="AB1128" s="10">
+        <v>84.6</v>
+      </c>
+      <c r="AC1128" s="10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1129" spans="1:29" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1129" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1129" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1129" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1129" s="7">
+        <v>100</v>
+      </c>
+      <c r="F1129" s="7">
+        <v>67.3</v>
+      </c>
+      <c r="G1129" s="7">
+        <v>6.1</v>
+      </c>
+      <c r="H1129" s="7">
+        <v>100</v>
+      </c>
+      <c r="I1129" s="7">
+        <v>100</v>
+      </c>
+      <c r="J1129" s="7">
+        <v>77.400000000000006</v>
+      </c>
+      <c r="K1129" s="7">
+        <v>12</v>
+      </c>
+      <c r="L1129" s="7">
+        <v>92</v>
+      </c>
+      <c r="M1129" s="7">
+        <v>10</v>
+      </c>
+      <c r="T1129" s="7">
+        <v>62.3</v>
+      </c>
+      <c r="U1129" s="7">
+        <v>56</v>
+      </c>
+      <c r="V1129" s="7">
+        <v>75.8</v>
+      </c>
+      <c r="W1129" s="7">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1130" spans="1:29" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1130" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1130" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1130" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1130" s="7">
+        <v>100</v>
+      </c>
+      <c r="F1130" s="7">
+        <v>67.900000000000006</v>
+      </c>
+      <c r="G1130" s="7">
+        <v>83.7</v>
+      </c>
+      <c r="H1130" s="7">
+        <v>0</v>
+      </c>
+      <c r="I1130" s="7">
+        <v>0</v>
+      </c>
+      <c r="J1130" s="7">
+        <v>76.7</v>
+      </c>
+      <c r="K1130" s="7">
+        <v>27</v>
+      </c>
+      <c r="L1130" s="7">
+        <v>87.5</v>
+      </c>
+      <c r="M1130" s="7">
+        <v>18</v>
+      </c>
+      <c r="N1130" s="7">
+        <v>95</v>
+      </c>
+      <c r="O1130" s="7">
+        <v>18</v>
+      </c>
+      <c r="P1130" s="7">
+        <v>100</v>
+      </c>
+      <c r="Q1130" s="7">
+        <v>10</v>
+      </c>
+      <c r="R1130" s="7">
+        <v>100</v>
+      </c>
+      <c r="S1130" s="7">
+        <v>10</v>
+      </c>
+      <c r="T1130" s="7">
+        <v>75.900000000000006</v>
+      </c>
+      <c r="U1130" s="7">
+        <v>13</v>
+      </c>
+      <c r="V1130" s="7">
+        <v>81</v>
+      </c>
+      <c r="W1130" s="7">
+        <v>10</v>
+      </c>
+      <c r="X1130" s="7">
+        <v>91.3</v>
+      </c>
+      <c r="Y1130" s="7">
+        <v>10</v>
+      </c>
+      <c r="Z1130" s="7">
+        <v>85.2</v>
+      </c>
+      <c r="AA1130" s="7">
+        <v>12</v>
+      </c>
+      <c r="AB1130" s="7">
+        <v>85.7</v>
+      </c>
+      <c r="AC1130" s="7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1131" spans="1:29" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1131" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1131" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1131" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1131" s="7">
+        <v>100</v>
+      </c>
+      <c r="F1131" s="7">
+        <v>63.3</v>
+      </c>
+      <c r="G1131" s="7">
+        <v>29.9</v>
+      </c>
+      <c r="H1131" s="7">
+        <v>100</v>
+      </c>
+      <c r="I1131" s="7">
+        <v>100</v>
+      </c>
+      <c r="J1131" s="7">
+        <v>69.099999999999994</v>
+      </c>
+      <c r="K1131" s="7">
+        <v>31</v>
+      </c>
+      <c r="L1131" s="7">
+        <v>95.5</v>
+      </c>
+      <c r="M1131" s="7">
+        <v>10</v>
+      </c>
+      <c r="N1131" s="7">
+        <v>87.5</v>
+      </c>
+      <c r="O1131" s="7">
+        <v>11</v>
+      </c>
+      <c r="T1131" s="7">
+        <v>60</v>
+      </c>
+      <c r="U1131" s="7">
+        <v>57</v>
+      </c>
+      <c r="V1131" s="7">
+        <v>76.5</v>
+      </c>
+      <c r="W1131" s="7">
+        <v>15</v>
+      </c>
+      <c r="X1131" s="7">
+        <v>81</v>
+      </c>
+      <c r="Y1131" s="7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1132" spans="1:29" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1132" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="B1132" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1132" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1132" s="7">
+        <v>98.9</v>
+      </c>
+      <c r="F1132" s="7">
+        <v>70.2</v>
+      </c>
+      <c r="G1132" s="7">
+        <v>74.599999999999994</v>
+      </c>
+      <c r="H1132" s="7">
+        <v>0</v>
+      </c>
+      <c r="I1132" s="7">
+        <v>0</v>
+      </c>
+      <c r="J1132" s="7">
+        <v>75</v>
+      </c>
+      <c r="K1132" s="7">
+        <v>43</v>
+      </c>
+      <c r="L1132" s="7">
+        <v>89.3</v>
+      </c>
+      <c r="M1132" s="7">
+        <v>11</v>
+      </c>
+      <c r="N1132" s="7">
+        <v>91.2</v>
+      </c>
+      <c r="O1132" s="7">
+        <v>13</v>
+      </c>
+      <c r="P1132" s="7">
+        <v>96.8</v>
+      </c>
+      <c r="Q1132" s="7">
+        <v>12</v>
+      </c>
+      <c r="R1132" s="7">
+        <v>100</v>
+      </c>
+      <c r="S1132" s="7">
+        <v>10</v>
+      </c>
+      <c r="T1132" s="7">
+        <v>87.1</v>
+      </c>
+      <c r="U1132" s="7">
+        <v>12</v>
+      </c>
+      <c r="V1132" s="7">
+        <v>89.3</v>
+      </c>
+      <c r="W1132" s="7">
+        <v>11</v>
+      </c>
+      <c r="X1132" s="7">
+        <v>93.3</v>
+      </c>
+      <c r="Y1132" s="7">
+        <v>12</v>
+      </c>
+      <c r="Z1132" s="7">
         <v>92.9</v>
       </c>
-      <c r="M1116">
+      <c r="AA1132" s="7">
+        <v>11</v>
+      </c>
+      <c r="AB1132" s="7">
+        <v>88.5</v>
+      </c>
+      <c r="AC1132" s="7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1133" spans="1:29" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1133" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="B1133" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1133" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1133" s="13">
+        <v>100</v>
+      </c>
+      <c r="F1133" s="13">
+        <v>69.400000000000006</v>
+      </c>
+      <c r="G1133" s="13">
+        <v>29</v>
+      </c>
+      <c r="H1133" s="13">
+        <v>100</v>
+      </c>
+      <c r="I1133" s="13">
+        <v>100</v>
+      </c>
+      <c r="J1133" s="13">
+        <v>73.8</v>
+      </c>
+      <c r="K1133" s="13">
+        <v>24</v>
+      </c>
+      <c r="L1133" s="13">
+        <v>89.3</v>
+      </c>
+      <c r="M1133" s="13">
+        <v>11</v>
+      </c>
+      <c r="N1133" s="13">
+        <v>94.3</v>
+      </c>
+      <c r="O1133" s="13">
+        <v>14</v>
+      </c>
+      <c r="P1133" s="13">
+        <v>75</v>
+      </c>
+      <c r="Q1133" s="13">
+        <v>10</v>
+      </c>
+      <c r="T1133" s="13">
+        <v>79.099999999999994</v>
+      </c>
+      <c r="U1133" s="13">
+        <v>17</v>
+      </c>
+      <c r="V1133" s="13">
+        <v>94.7</v>
+      </c>
+      <c r="W1133" s="13">
+        <v>15</v>
+      </c>
+      <c r="X1133" s="13">
+        <v>79.2</v>
+      </c>
+      <c r="Y1133" s="13">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1134" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1134" t="s">
+        <v>83</v>
+      </c>
+      <c r="B1134" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1134" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1134">
+        <v>97</v>
+      </c>
+      <c r="F1134">
+        <v>74.5</v>
+      </c>
+      <c r="G1134">
+        <v>79.2</v>
+      </c>
+      <c r="H1134">
+        <v>0</v>
+      </c>
+      <c r="I1134">
+        <v>0</v>
+      </c>
+      <c r="J1134">
+        <v>77.900000000000006</v>
+      </c>
+      <c r="K1134">
+        <v>32</v>
+      </c>
+      <c r="L1134">
+        <v>85.5</v>
+      </c>
+      <c r="M1134">
+        <v>27</v>
+      </c>
+      <c r="N1134">
+        <v>96.1</v>
+      </c>
+      <c r="O1134">
+        <v>12</v>
+      </c>
+      <c r="P1134">
+        <v>98</v>
+      </c>
+      <c r="Q1134">
+        <v>12</v>
+      </c>
+      <c r="R1134">
+        <v>97.6</v>
+      </c>
+      <c r="S1134">
+        <v>10</v>
+      </c>
+      <c r="T1134">
+        <v>81.7</v>
+      </c>
+      <c r="U1134">
+        <v>29</v>
+      </c>
+      <c r="V1134">
+        <v>86.4</v>
+      </c>
+      <c r="W1134">
+        <v>14</v>
+      </c>
+      <c r="X1134">
+        <v>93</v>
+      </c>
+      <c r="Y1134">
+        <v>13</v>
+      </c>
+      <c r="Z1134">
+        <v>95.7</v>
+      </c>
+      <c r="AA1134">
+        <v>11</v>
+      </c>
+      <c r="AB1134">
+        <v>95.9</v>
+      </c>
+      <c r="AC1134">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1135" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1135" t="s">
+        <v>83</v>
+      </c>
+      <c r="B1135" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1135" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1135">
+        <v>100</v>
+      </c>
+      <c r="F1135">
+        <v>72.7</v>
+      </c>
+      <c r="G1135">
+        <v>54.4</v>
+      </c>
+      <c r="H1135">
+        <v>100</v>
+      </c>
+      <c r="I1135">
+        <v>100</v>
+      </c>
+      <c r="J1135">
+        <v>84.4</v>
+      </c>
+      <c r="K1135">
+        <v>18</v>
+      </c>
+      <c r="L1135">
+        <v>82.9</v>
+      </c>
+      <c r="M1135">
+        <v>10</v>
+      </c>
+      <c r="N1135">
+        <v>87.5</v>
+      </c>
+      <c r="O1135">
+        <v>15</v>
+      </c>
+      <c r="P1135">
+        <v>93.3</v>
+      </c>
+      <c r="Q1135">
+        <v>11</v>
+      </c>
+      <c r="S1135"/>
+      <c r="T1135">
+        <v>77.099999999999994</v>
+      </c>
+      <c r="U1135">
+        <v>33</v>
+      </c>
+      <c r="V1135">
+        <v>85.5</v>
+      </c>
+      <c r="W1135">
         <v>19</v>
       </c>
-      <c r="N1116">
-        <v>91.7</v>
-      </c>
-      <c r="O1116">
-        <v>17</v>
-      </c>
-      <c r="P1116">
-        <v>92.9</v>
-      </c>
-      <c r="Q1116">
-        <v>19</v>
-      </c>
-      <c r="R1116">
-        <v>94.7</v>
-      </c>
-      <c r="S1116">
-        <v>26</v>
-      </c>
-      <c r="T1116">
-        <v>91.7</v>
-      </c>
-      <c r="U1116">
-        <v>17</v>
-      </c>
-      <c r="V1116">
-        <v>100</v>
-      </c>
-      <c r="W1116">
-        <v>10</v>
-      </c>
-      <c r="X1116">
-        <v>100</v>
-      </c>
-      <c r="Y1116">
-        <v>14</v>
-      </c>
-      <c r="Z1116">
-        <v>100</v>
-      </c>
-      <c r="AA1116">
-        <v>10</v>
-      </c>
-      <c r="AB1116">
-        <v>100</v>
-      </c>
-      <c r="AC1116">
+      <c r="X1135">
+        <v>88.9</v>
+      </c>
+      <c r="Y1135">
         <v>11</v>
       </c>
-    </row>
-    <row r="1117" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A1117" t="s">
-        <v>74</v>
-      </c>
-      <c r="B1117" t="s">
-        <v>25</v>
-      </c>
-      <c r="D1117" t="s">
-        <v>30</v>
-      </c>
-      <c r="E1117">
-        <v>100</v>
-      </c>
-      <c r="F1117">
-        <v>69.400000000000006</v>
-      </c>
-      <c r="G1117">
-        <v>4.2</v>
-      </c>
-      <c r="H1117">
-        <v>100</v>
-      </c>
-      <c r="I1117">
-        <v>100</v>
-      </c>
-      <c r="J1117">
-        <v>100</v>
-      </c>
-      <c r="K1117">
-        <v>10</v>
-      </c>
-      <c r="L1117">
-        <v>100</v>
-      </c>
-      <c r="M1117">
-        <v>11</v>
-      </c>
-      <c r="S1117"/>
-      <c r="T1117">
-        <v>72</v>
-      </c>
-      <c r="U1117">
-        <v>35</v>
-      </c>
-      <c r="V1117">
-        <v>87.5</v>
-      </c>
-      <c r="W1117">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="1118" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A1118" t="s">
-        <v>75</v>
-      </c>
-      <c r="B1118" t="s">
-        <v>25</v>
-      </c>
-      <c r="D1118" t="s">
-        <v>61</v>
-      </c>
-      <c r="E1118">
-        <v>100</v>
-      </c>
-      <c r="F1118">
-        <v>83.3</v>
-      </c>
-      <c r="G1118">
-        <v>98.3</v>
-      </c>
-      <c r="H1118">
-        <v>0</v>
-      </c>
-      <c r="I1118">
-        <v>0</v>
-      </c>
-      <c r="J1118">
-        <v>100</v>
-      </c>
-      <c r="K1118">
-        <v>17</v>
-      </c>
-      <c r="L1118">
-        <v>100</v>
-      </c>
-      <c r="M1118">
-        <v>17</v>
-      </c>
-      <c r="N1118">
-        <v>100</v>
-      </c>
-      <c r="O1118">
-        <v>17</v>
-      </c>
-      <c r="P1118">
-        <v>100</v>
-      </c>
-      <c r="Q1118">
-        <v>17</v>
-      </c>
-      <c r="R1118">
-        <v>100</v>
-      </c>
-      <c r="S1118">
-        <v>17</v>
-      </c>
-      <c r="T1118">
-        <v>88.2</v>
-      </c>
-      <c r="U1118">
-        <v>28</v>
-      </c>
-      <c r="V1118">
-        <v>92.3</v>
-      </c>
-      <c r="W1118">
-        <v>22</v>
-      </c>
-      <c r="X1118">
-        <v>100</v>
-      </c>
-      <c r="Y1118">
-        <v>10</v>
-      </c>
-      <c r="Z1118">
-        <v>90.9</v>
-      </c>
-      <c r="AA1118">
-        <v>18</v>
-      </c>
-      <c r="AB1118">
-        <v>92.9</v>
-      </c>
-      <c r="AC1118">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="1119" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A1119" t="s">
-        <v>75</v>
-      </c>
-      <c r="B1119" t="s">
-        <v>25</v>
-      </c>
-      <c r="D1119" t="s">
-        <v>30</v>
-      </c>
-      <c r="E1119">
-        <v>100</v>
-      </c>
-      <c r="F1119">
-        <v>76.7</v>
-      </c>
-      <c r="G1119">
-        <v>33.299999999999997</v>
-      </c>
-      <c r="H1119">
-        <v>100</v>
-      </c>
-      <c r="I1119">
-        <v>100</v>
-      </c>
-      <c r="J1119">
-        <v>77.3</v>
-      </c>
-      <c r="K1119">
-        <v>37</v>
-      </c>
-      <c r="L1119">
-        <v>100</v>
-      </c>
-      <c r="M1119">
-        <v>10</v>
-      </c>
-      <c r="N1119">
-        <v>100</v>
-      </c>
-      <c r="O1119">
-        <v>13</v>
-      </c>
-      <c r="S1119"/>
-      <c r="T1119">
-        <v>87.5</v>
-      </c>
-      <c r="U1119">
-        <v>40</v>
-      </c>
-      <c r="V1119">
-        <v>91.7</v>
-      </c>
-      <c r="W1119">
-        <v>20</v>
-      </c>
-      <c r="X1119">
-        <v>87.5</v>
-      </c>
-      <c r="Y1119">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="1120" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A1120" t="s">
-        <v>76</v>
-      </c>
-      <c r="B1120" t="s">
-        <v>25</v>
-      </c>
-      <c r="D1120" t="s">
-        <v>61</v>
-      </c>
-      <c r="E1120">
-        <v>98.4</v>
-      </c>
-      <c r="F1120">
-        <v>80.3</v>
-      </c>
-      <c r="G1120">
-        <v>97</v>
-      </c>
-      <c r="H1120">
-        <v>0</v>
-      </c>
-      <c r="I1120">
-        <v>0</v>
-      </c>
-      <c r="J1120">
-        <v>100</v>
-      </c>
-      <c r="K1120">
-        <v>24</v>
-      </c>
-      <c r="L1120">
-        <v>100</v>
-      </c>
-      <c r="M1120">
-        <v>23</v>
-      </c>
-      <c r="N1120">
-        <v>100</v>
-      </c>
-      <c r="O1120">
-        <v>20</v>
-      </c>
-      <c r="P1120">
-        <v>100</v>
-      </c>
-      <c r="Q1120">
-        <v>14</v>
-      </c>
-      <c r="R1120">
-        <v>100</v>
-      </c>
-      <c r="S1120">
-        <v>14</v>
-      </c>
-      <c r="T1120">
-        <v>85.7</v>
-      </c>
-      <c r="U1120">
-        <v>21</v>
-      </c>
-      <c r="V1120">
-        <v>87.5</v>
-      </c>
-      <c r="W1120">
+      <c r="Z1135">
+        <v>90.2</v>
+      </c>
+      <c r="AA1135">
         <v>12</v>
-      </c>
-      <c r="X1120">
-        <v>87.5</v>
-      </c>
-      <c r="Y1120">
-        <v>12</v>
-      </c>
-      <c r="Z1120">
-        <v>90</v>
-      </c>
-      <c r="AA1120">
-        <v>15</v>
-      </c>
-      <c r="AB1120">
-        <v>100</v>
-      </c>
-      <c r="AC1120">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="1121" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A1121" t="s">
-        <v>76</v>
-      </c>
-      <c r="B1121" t="s">
-        <v>25</v>
-      </c>
-      <c r="D1121" t="s">
-        <v>30</v>
-      </c>
-      <c r="E1121">
-        <v>100</v>
-      </c>
-      <c r="F1121">
-        <v>77.3</v>
-      </c>
-      <c r="G1121">
-        <v>69.7</v>
-      </c>
-      <c r="H1121">
-        <v>100</v>
-      </c>
-      <c r="I1121">
-        <v>100</v>
-      </c>
-      <c r="J1121">
-        <v>100</v>
-      </c>
-      <c r="K1121">
-        <v>12</v>
-      </c>
-      <c r="L1121">
-        <v>100</v>
-      </c>
-      <c r="M1121">
-        <v>24</v>
-      </c>
-      <c r="N1121">
-        <v>100</v>
-      </c>
-      <c r="O1121">
-        <v>11</v>
-      </c>
-      <c r="P1121">
-        <v>100</v>
-      </c>
-      <c r="Q1121">
-        <v>11</v>
-      </c>
-      <c r="R1121">
-        <v>71.400000000000006</v>
-      </c>
-      <c r="S1121">
-        <v>11</v>
-      </c>
-      <c r="T1121">
-        <v>71.400000000000006</v>
-      </c>
-      <c r="U1121">
-        <v>21</v>
-      </c>
-      <c r="V1121">
-        <v>80</v>
-      </c>
-      <c r="W1121">
-        <v>23</v>
-      </c>
-      <c r="X1121">
-        <v>88.9</v>
-      </c>
-      <c r="Y1121">
-        <v>14</v>
-      </c>
-      <c r="Z1121">
-        <v>88.9</v>
-      </c>
-      <c r="AA1121">
-        <v>14</v>
-      </c>
-      <c r="AB1121">
-        <v>85.7</v>
-      </c>
-      <c r="AC1121">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="1122" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A1122" t="s">
-        <v>77</v>
-      </c>
-      <c r="B1122" t="s">
-        <v>25</v>
-      </c>
-      <c r="D1122" t="s">
-        <v>61</v>
-      </c>
-      <c r="E1122">
-        <v>100</v>
-      </c>
-      <c r="F1122">
-        <v>61.4</v>
-      </c>
-      <c r="G1122">
-        <v>82.2</v>
-      </c>
-      <c r="H1122">
-        <v>0</v>
-      </c>
-      <c r="I1122">
-        <v>0</v>
-      </c>
-      <c r="J1122">
-        <v>69.599999999999994</v>
-      </c>
-      <c r="K1122">
-        <v>19</v>
-      </c>
-      <c r="L1122">
-        <v>74.5</v>
-      </c>
-      <c r="M1122">
-        <v>10</v>
-      </c>
-      <c r="N1122">
-        <v>73.8</v>
-      </c>
-      <c r="O1122">
-        <v>16</v>
-      </c>
-      <c r="P1122">
-        <v>78.8</v>
-      </c>
-      <c r="Q1122">
-        <v>11</v>
-      </c>
-      <c r="R1122">
-        <v>73.099999999999994</v>
-      </c>
-      <c r="S1122">
-        <v>11</v>
-      </c>
-      <c r="T1122">
-        <v>69.2</v>
-      </c>
-      <c r="U1122">
-        <v>16</v>
-      </c>
-      <c r="V1122">
-        <v>74.5</v>
-      </c>
-      <c r="W1122">
-        <v>11</v>
-      </c>
-      <c r="X1122">
-        <v>78</v>
-      </c>
-      <c r="Y1122">
-        <v>12</v>
-      </c>
-      <c r="Z1122">
-        <v>78.2</v>
-      </c>
-      <c r="AA1122">
-        <v>11</v>
-      </c>
-      <c r="AB1122">
-        <v>75</v>
-      </c>
-      <c r="AC1122">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="1123" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A1123" t="s">
-        <v>77</v>
-      </c>
-      <c r="B1123" t="s">
-        <v>25</v>
-      </c>
-      <c r="D1123" t="s">
-        <v>30</v>
-      </c>
-      <c r="E1123">
-        <v>100</v>
-      </c>
-      <c r="F1123">
-        <v>60.8</v>
-      </c>
-      <c r="G1123">
-        <v>24.8</v>
-      </c>
-      <c r="H1123">
-        <v>100</v>
-      </c>
-      <c r="I1123">
-        <v>100</v>
-      </c>
-      <c r="J1123">
-        <v>71.2</v>
-      </c>
-      <c r="K1123">
-        <v>11</v>
-      </c>
-      <c r="L1123">
-        <v>72.7</v>
-      </c>
-      <c r="M1123">
-        <v>13</v>
-      </c>
-      <c r="N1123">
-        <v>64.099999999999994</v>
-      </c>
-      <c r="O1123">
-        <v>19</v>
-      </c>
-      <c r="S1123"/>
-      <c r="T1123">
-        <v>58.7</v>
-      </c>
-      <c r="U1123">
-        <v>43</v>
-      </c>
-      <c r="V1123">
-        <v>69.3</v>
-      </c>
-      <c r="W1123">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="1124" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A1124" t="s">
-        <v>78</v>
-      </c>
-      <c r="B1124" t="s">
-        <v>25</v>
-      </c>
-      <c r="D1124" t="s">
-        <v>61</v>
-      </c>
-      <c r="E1124">
-        <v>100</v>
-      </c>
-      <c r="F1124">
-        <v>66.3</v>
-      </c>
-      <c r="G1124">
-        <v>78.099999999999994</v>
-      </c>
-      <c r="H1124">
-        <v>0</v>
-      </c>
-      <c r="I1124">
-        <v>0</v>
-      </c>
-      <c r="J1124">
-        <v>65.900000000000006</v>
-      </c>
-      <c r="K1124">
-        <v>32</v>
-      </c>
-      <c r="L1124">
-        <v>67.8</v>
-      </c>
-      <c r="M1124">
-        <v>43</v>
-      </c>
-      <c r="N1124">
-        <v>81</v>
-      </c>
-      <c r="O1124">
-        <v>10</v>
-      </c>
-      <c r="P1124">
-        <v>74.2</v>
-      </c>
-      <c r="Q1124">
-        <v>16</v>
-      </c>
-      <c r="R1124">
-        <v>78.3</v>
-      </c>
-      <c r="S1124">
-        <v>11</v>
-      </c>
-      <c r="T1124">
-        <v>73.3</v>
-      </c>
-      <c r="U1124">
-        <v>24</v>
-      </c>
-      <c r="V1124">
-        <v>79.3</v>
-      </c>
-      <c r="W1124">
-        <v>14</v>
-      </c>
-      <c r="X1124">
-        <v>87.2</v>
-      </c>
-      <c r="Y1124">
-        <v>11</v>
-      </c>
-      <c r="Z1124">
-        <v>83.7</v>
-      </c>
-      <c r="AA1124">
-        <v>10</v>
-      </c>
-      <c r="AB1124">
-        <v>84.4</v>
-      </c>
-      <c r="AC1124">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="1125" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A1125" t="s">
-        <v>78</v>
-      </c>
-      <c r="B1125" t="s">
-        <v>25</v>
-      </c>
-      <c r="D1125" t="s">
-        <v>30</v>
-      </c>
-      <c r="E1125">
-        <v>100</v>
-      </c>
-      <c r="F1125">
-        <v>62.5</v>
-      </c>
-      <c r="G1125">
-        <v>49.8</v>
-      </c>
-      <c r="H1125">
-        <v>100</v>
-      </c>
-      <c r="I1125">
-        <v>100</v>
-      </c>
-      <c r="J1125">
-        <v>62.5</v>
-      </c>
-      <c r="K1125">
-        <v>52</v>
-      </c>
-      <c r="L1125">
-        <v>67.099999999999994</v>
-      </c>
-      <c r="M1125">
-        <v>35</v>
-      </c>
-      <c r="N1125">
-        <v>70.900000000000006</v>
-      </c>
-      <c r="O1125">
-        <v>13</v>
-      </c>
-      <c r="P1125">
-        <v>65.8</v>
-      </c>
-      <c r="Q1125">
-        <v>18</v>
-      </c>
-      <c r="S1125"/>
-      <c r="T1125">
-        <v>69.099999999999994</v>
-      </c>
-      <c r="U1125">
-        <v>33</v>
-      </c>
-      <c r="V1125">
-        <v>83.7</v>
-      </c>
-      <c r="W1125">
-        <v>12</v>
-      </c>
-      <c r="X1125">
-        <v>81</v>
-      </c>
-      <c r="Y1125">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="1126" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A1126" t="s">
-        <v>79</v>
-      </c>
-      <c r="B1126" t="s">
-        <v>25</v>
-      </c>
-      <c r="D1126" t="s">
-        <v>61</v>
-      </c>
-      <c r="E1126">
-        <v>99</v>
-      </c>
-      <c r="F1126">
-        <v>68.400000000000006</v>
-      </c>
-      <c r="G1126">
-        <v>86.3</v>
-      </c>
-      <c r="H1126">
-        <v>0</v>
-      </c>
-      <c r="I1126">
-        <v>0</v>
-      </c>
-      <c r="J1126">
-        <v>68.7</v>
-      </c>
-      <c r="K1126">
-        <v>32</v>
-      </c>
-      <c r="L1126">
-        <v>71.400000000000006</v>
-      </c>
-      <c r="M1126">
-        <v>41</v>
-      </c>
-      <c r="N1126">
-        <v>77.2</v>
-      </c>
-      <c r="O1126">
-        <v>12</v>
-      </c>
-      <c r="P1126">
-        <v>78.599999999999994</v>
-      </c>
-      <c r="Q1126">
-        <v>34</v>
-      </c>
-      <c r="R1126">
-        <v>86.5</v>
-      </c>
-      <c r="S1126">
-        <v>16</v>
-      </c>
-      <c r="T1126">
-        <v>75.400000000000006</v>
-      </c>
-      <c r="U1126">
-        <v>14</v>
-      </c>
-      <c r="V1126">
-        <v>82.4</v>
-      </c>
-      <c r="W1126">
-        <v>18</v>
-      </c>
-      <c r="X1126">
-        <v>84.9</v>
-      </c>
-      <c r="Y1126">
-        <v>11</v>
-      </c>
-      <c r="Z1126">
-        <v>85.7</v>
-      </c>
-      <c r="AA1126">
-        <v>12</v>
-      </c>
-      <c r="AB1126">
-        <v>83.3</v>
-      </c>
-      <c r="AC1126">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="1127" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A1127" t="s">
-        <v>79</v>
-      </c>
-      <c r="B1127" t="s">
-        <v>25</v>
-      </c>
-      <c r="D1127" t="s">
-        <v>30</v>
-      </c>
-      <c r="E1127">
-        <v>100</v>
-      </c>
-      <c r="F1127">
-        <v>66.7</v>
-      </c>
-      <c r="G1127">
-        <v>100</v>
-      </c>
-      <c r="H1127">
-        <v>100</v>
-      </c>
-      <c r="I1127">
-        <v>100</v>
-      </c>
-      <c r="J1127">
-        <v>65.3</v>
-      </c>
-      <c r="K1127">
-        <v>61</v>
-      </c>
-      <c r="L1127">
-        <v>67.599999999999994</v>
-      </c>
-      <c r="M1127">
-        <v>40</v>
-      </c>
-      <c r="N1127">
-        <v>67.599999999999994</v>
-      </c>
-      <c r="O1127">
-        <v>14</v>
-      </c>
-      <c r="P1127">
-        <v>61.7</v>
-      </c>
-      <c r="Q1127">
-        <v>13</v>
-      </c>
-      <c r="R1127">
-        <v>63.4</v>
-      </c>
-      <c r="S1127">
-        <v>17</v>
-      </c>
-      <c r="T1127">
-        <v>69.900000000000006</v>
-      </c>
-      <c r="U1127">
-        <v>39</v>
-      </c>
-      <c r="V1127">
-        <v>73.7</v>
-      </c>
-      <c r="W1127">
-        <v>21</v>
-      </c>
-      <c r="X1127">
-        <v>73.900000000000006</v>
-      </c>
-      <c r="Y1127">
-        <v>10</v>
-      </c>
-      <c r="Z1127">
-        <v>74.599999999999994</v>
-      </c>
-      <c r="AA1127">
-        <v>12</v>
-      </c>
-      <c r="AB1127">
-        <v>73.900000000000006</v>
-      </c>
-      <c r="AC1127">
-        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
dodałem statystykę Tr_cnt do excela
</commit_message>
<xml_diff>
--- a/wm/Results.xlsx
+++ b/wm/Results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pioo\notebooks\wm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BB3ABC8-25AA-418F-B054-7AD5F6F1B73A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67E1D664-8CF1-4FCF-A7BB-384BB6B7D71B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="330" yWindow="780" windowWidth="28470" windowHeight="11340" tabRatio="435" xr2:uid="{B6B0453F-83A4-43EC-A328-DC10FEB5BD2E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="435" xr2:uid="{B6B0453F-83A4-43EC-A328-DC10FEB5BD2E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3437" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3452" uniqueCount="90">
   <si>
     <t>Te_cal</t>
   </si>
@@ -292,6 +292,21 @@
   </si>
   <si>
     <t>test26_16c</t>
+  </si>
+  <si>
+    <t>test27_16c</t>
+  </si>
+  <si>
+    <t>test28_16c precision</t>
+  </si>
+  <si>
+    <t>test28_16c accuracy</t>
+  </si>
+  <si>
+    <t>test29_16c precision</t>
+  </si>
+  <si>
+    <t>test29_16c accuracy</t>
   </si>
 </sst>
 </file>
@@ -755,13 +770,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBA71D6A-A9B1-42AC-9396-7E4A540CDDDA}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:AC1137"/>
+  <dimension ref="A1:AC1142"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="4" ySplit="1" topLeftCell="E1112" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E1138" sqref="E1138"/>
+      <selection pane="bottomRight" activeCell="A1137" sqref="A1137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -88177,6 +88192,430 @@
       </c>
       <c r="AC1137">
         <v>13</v>
+      </c>
+    </row>
+    <row r="1138" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1138" t="s">
+        <v>85</v>
+      </c>
+      <c r="B1138" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1138" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1138">
+        <v>96.9</v>
+      </c>
+      <c r="F1138">
+        <v>92</v>
+      </c>
+      <c r="G1138">
+        <v>94.9</v>
+      </c>
+      <c r="H1138">
+        <v>0</v>
+      </c>
+      <c r="I1138">
+        <v>0</v>
+      </c>
+      <c r="J1138">
+        <v>99.4</v>
+      </c>
+      <c r="K1138">
+        <v>38</v>
+      </c>
+      <c r="L1138">
+        <v>99.8</v>
+      </c>
+      <c r="M1138">
+        <v>24</v>
+      </c>
+      <c r="N1138">
+        <v>99.9</v>
+      </c>
+      <c r="O1138">
+        <v>10</v>
+      </c>
+      <c r="P1138">
+        <v>100</v>
+      </c>
+      <c r="Q1138">
+        <v>17</v>
+      </c>
+      <c r="R1138">
+        <v>100</v>
+      </c>
+      <c r="S1138">
+        <v>10</v>
+      </c>
+      <c r="T1138">
+        <v>12.3</v>
+      </c>
+      <c r="U1138">
+        <v>11</v>
+      </c>
+      <c r="V1138">
+        <v>13.7</v>
+      </c>
+      <c r="W1138">
+        <v>10</v>
+      </c>
+      <c r="X1138">
+        <v>14.4</v>
+      </c>
+      <c r="Y1138">
+        <v>10</v>
+      </c>
+      <c r="Z1138">
+        <v>14.2</v>
+      </c>
+      <c r="AA1138">
+        <v>10</v>
+      </c>
+      <c r="AB1138">
+        <v>10.8</v>
+      </c>
+      <c r="AC1138">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1139" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1139" t="s">
+        <v>86</v>
+      </c>
+      <c r="B1139" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1139" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1139">
+        <v>99</v>
+      </c>
+      <c r="F1139">
+        <v>95.2</v>
+      </c>
+      <c r="G1139">
+        <v>96.2</v>
+      </c>
+      <c r="H1139">
+        <v>0</v>
+      </c>
+      <c r="I1139">
+        <v>0</v>
+      </c>
+      <c r="J1139">
+        <v>99.3</v>
+      </c>
+      <c r="K1139">
+        <v>34</v>
+      </c>
+      <c r="L1139">
+        <v>99.6</v>
+      </c>
+      <c r="M1139">
+        <v>21</v>
+      </c>
+      <c r="N1139">
+        <v>99.8</v>
+      </c>
+      <c r="O1139">
+        <v>12</v>
+      </c>
+      <c r="P1139">
+        <v>99.8</v>
+      </c>
+      <c r="Q1139">
+        <v>19</v>
+      </c>
+      <c r="R1139">
+        <v>99.6</v>
+      </c>
+      <c r="S1139">
+        <v>10</v>
+      </c>
+      <c r="T1139">
+        <v>12.3</v>
+      </c>
+      <c r="U1139">
+        <v>12</v>
+      </c>
+      <c r="V1139">
+        <v>12.3</v>
+      </c>
+      <c r="W1139">
+        <v>14</v>
+      </c>
+      <c r="X1139">
+        <v>12.1</v>
+      </c>
+      <c r="Y1139">
+        <v>12</v>
+      </c>
+      <c r="Z1139">
+        <v>12</v>
+      </c>
+      <c r="AA1139">
+        <v>11</v>
+      </c>
+      <c r="AB1139">
+        <v>10</v>
+      </c>
+      <c r="AC1139">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1140" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1140" t="s">
+        <v>87</v>
+      </c>
+      <c r="B1140" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1140" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1140">
+        <v>99</v>
+      </c>
+      <c r="F1140">
+        <v>96</v>
+      </c>
+      <c r="G1140">
+        <v>97.2</v>
+      </c>
+      <c r="H1140">
+        <v>0</v>
+      </c>
+      <c r="I1140">
+        <v>0</v>
+      </c>
+      <c r="J1140">
+        <v>99.5</v>
+      </c>
+      <c r="K1140">
+        <v>28</v>
+      </c>
+      <c r="L1140">
+        <v>99.7</v>
+      </c>
+      <c r="M1140">
+        <v>15</v>
+      </c>
+      <c r="N1140">
+        <v>99.6</v>
+      </c>
+      <c r="O1140">
+        <v>15</v>
+      </c>
+      <c r="P1140">
+        <v>99.6</v>
+      </c>
+      <c r="Q1140">
+        <v>30</v>
+      </c>
+      <c r="R1140">
+        <v>99.8</v>
+      </c>
+      <c r="S1140">
+        <v>13</v>
+      </c>
+      <c r="T1140">
+        <v>12.1</v>
+      </c>
+      <c r="U1140">
+        <v>12</v>
+      </c>
+      <c r="V1140">
+        <v>12.9</v>
+      </c>
+      <c r="W1140">
+        <v>10</v>
+      </c>
+      <c r="X1140">
+        <v>12.7</v>
+      </c>
+      <c r="Y1140">
+        <v>10</v>
+      </c>
+      <c r="Z1140">
+        <v>12.5</v>
+      </c>
+      <c r="AA1140">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1141" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1141" t="s">
+        <v>88</v>
+      </c>
+      <c r="B1141" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1141" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1141">
+        <v>99.4</v>
+      </c>
+      <c r="F1141">
+        <v>94.9</v>
+      </c>
+      <c r="G1141">
+        <v>97.3</v>
+      </c>
+      <c r="H1141">
+        <v>0</v>
+      </c>
+      <c r="I1141">
+        <v>0</v>
+      </c>
+      <c r="J1141">
+        <v>99.6</v>
+      </c>
+      <c r="K1141">
+        <v>20</v>
+      </c>
+      <c r="L1141">
+        <v>99.7</v>
+      </c>
+      <c r="M1141">
+        <v>10</v>
+      </c>
+      <c r="N1141">
+        <v>99.6</v>
+      </c>
+      <c r="O1141">
+        <v>28</v>
+      </c>
+      <c r="P1141">
+        <v>99.7</v>
+      </c>
+      <c r="Q1141">
+        <v>17</v>
+      </c>
+      <c r="R1141">
+        <v>99.7</v>
+      </c>
+      <c r="S1141">
+        <v>13</v>
+      </c>
+      <c r="T1141">
+        <v>13.1</v>
+      </c>
+      <c r="U1141">
+        <v>10</v>
+      </c>
+      <c r="V1141">
+        <v>13.3</v>
+      </c>
+      <c r="W1141">
+        <v>10</v>
+      </c>
+      <c r="X1141">
+        <v>13.3</v>
+      </c>
+      <c r="Y1141">
+        <v>11</v>
+      </c>
+      <c r="Z1141">
+        <v>13.2</v>
+      </c>
+      <c r="AA1141">
+        <v>10</v>
+      </c>
+      <c r="AB1141">
+        <v>9.5</v>
+      </c>
+      <c r="AC1141">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1142" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1142" t="s">
+        <v>89</v>
+      </c>
+      <c r="B1142" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1142" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1142">
+        <v>99.5</v>
+      </c>
+      <c r="F1142">
+        <v>95.4</v>
+      </c>
+      <c r="G1142">
+        <v>97.5</v>
+      </c>
+      <c r="H1142">
+        <v>0</v>
+      </c>
+      <c r="I1142">
+        <v>0</v>
+      </c>
+      <c r="J1142">
+        <v>99.8</v>
+      </c>
+      <c r="K1142">
+        <v>16</v>
+      </c>
+      <c r="L1142">
+        <v>99.9</v>
+      </c>
+      <c r="M1142">
+        <v>11</v>
+      </c>
+      <c r="N1142">
+        <v>99.7</v>
+      </c>
+      <c r="O1142">
+        <v>25</v>
+      </c>
+      <c r="P1142">
+        <v>99.9</v>
+      </c>
+      <c r="Q1142">
+        <v>11</v>
+      </c>
+      <c r="R1142">
+        <v>99.8</v>
+      </c>
+      <c r="S1142">
+        <v>15</v>
+      </c>
+      <c r="T1142">
+        <v>13.6</v>
+      </c>
+      <c r="U1142">
+        <v>10</v>
+      </c>
+      <c r="V1142">
+        <v>13.7</v>
+      </c>
+      <c r="W1142">
+        <v>10</v>
+      </c>
+      <c r="X1142">
+        <v>13.1</v>
+      </c>
+      <c r="Y1142">
+        <v>10</v>
+      </c>
+      <c r="Z1142">
+        <v>13.7</v>
+      </c>
+      <c r="AA1142">
+        <v>10</v>
+      </c>
+      <c r="AB1142">
+        <v>12.9</v>
+      </c>
+      <c r="AC1142">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>